<commit_message>
Upgrade ClosedXML to 0.92.1 (#1)
* Upgrade ClosedXML to 0.92.1
* Upgrade projects to 2017 format
* Change target framework to 4.5
* Workbooks comparison improved to be version independent.
* Errors fixed
* Workaround for #686 introduced.
* Tests for pivot tables turned off since this feature looks non-finished
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Collapse.xlsx
+++ b/tests/Gauges/GroupTagTests_Collapse.xlsx
@@ -10,8 +10,8 @@
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="Orders">'Sheet1'!$A$12:$J$21</x:definedName>
-    <x:definedName name="Orders_tpl">'Sheet1'!$A$12:$J$13</x:definedName>
+    <x:definedName name="Orders">Sheet1!$A$12:$J$21</x:definedName>
+    <x:definedName name="Orders_tpl">Sheet1!$A$12:$J$13</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
@@ -303,7 +303,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="55">
+  <x:cellStyleXfs count="23">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -317,9 +317,6 @@
     <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -335,39 +332,24 @@
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -380,91 +362,13 @@
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -708,7 +612,7 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="3">
+  <x:dxfs count="1">
     <x:dxf>
       <x:font>
         <x:b val="0"/>
@@ -717,24 +621,6 @@
         <x:extend val="0"/>
         <x:color indexed="30"/>
       </x:font>
-    </x:dxf>
-    <x:dxf>
-      <x:font>
-        <x:color indexed="30"/>
-      </x:font>
-      <x:fill>
-        <x:patternFill/>
-      </x:fill>
-      <x:border/>
-    </x:dxf>
-    <x:dxf>
-      <x:font>
-        <x:color indexed="30"/>
-      </x:font>
-      <x:fill>
-        <x:patternFill patternType="solid"/>
-      </x:fill>
-      <x:border/>
     </x:dxf>
   </x:dxfs>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -813,45 +699,38 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>647701</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>629177</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="1695450" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2" descr="logo.png"/>
+        <xdr:cNvPr id="1" name="Рисунок 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2886075" y="19050"/>
-          <a:ext cx="1695451" cy="610127"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1695450" cy="609600"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1226,9 +1105,10 @@
     <x:col min="8" max="8" width="9.164062" style="45" customWidth="1"/>
     <x:col min="9" max="9" width="7.332031" style="45" customWidth="1"/>
     <x:col min="10" max="10" width="11.5" style="45" customWidth="1"/>
+    <x:col min="11" max="11" width="9.140625" style="45" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:10" customFormat="1" ht="51" customHeight="1">
+    <x:row r="1" spans="1:11" customFormat="1" ht="51" customHeight="1">
       <x:c r="A1" s="45" t="s"/>
       <x:c r="B1" s="46" t="s">
         <x:v>0</x:v>
@@ -1242,7 +1122,7 @@
       <x:c r="I1" s="47" t="s"/>
       <x:c r="J1" s="47" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:10" customFormat="1" ht="12.75" customHeight="1">
+    <x:row r="2" spans="1:11" customFormat="1" ht="12.75" customHeight="1">
       <x:c r="A2" s="45" t="s"/>
       <x:c r="B2" s="48" t="s"/>
       <x:c r="C2" s="48" t="s"/>
@@ -1254,7 +1134,7 @@
       <x:c r="I2" s="48" t="s"/>
       <x:c r="J2" s="45" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:10" customFormat="1" ht="18" customHeight="1">
+    <x:row r="3" spans="1:11" customFormat="1" ht="18" customHeight="1">
       <x:c r="A3" s="49" t="s"/>
       <x:c r="B3" s="50" t="s">
         <x:v>1</x:v>
@@ -1270,7 +1150,7 @@
       <x:c r="I3" s="53" t="s"/>
       <x:c r="J3" s="54" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:10">
+    <x:row r="4" spans="1:11">
       <x:c r="A4" s="45" t="s"/>
       <x:c r="B4" s="55" t="s"/>
       <x:c r="C4" s="45" t="s"/>
@@ -1282,14 +1162,14 @@
       <x:c r="I4" s="45" t="s"/>
       <x:c r="J4" s="45" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:10">
+    <x:row r="5" spans="1:11">
       <x:c r="A5" s="45" t="s"/>
       <x:c r="B5" s="50" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C5" s="45" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="6" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A6" s="45" t="s"/>
       <x:c r="B6" s="56" t="s">
         <x:f>"4-976 Sugarloaf Hwy"&amp;" "&amp;"Suite 103"</x:f>
@@ -1303,7 +1183,7 @@
       <x:c r="I6" s="59" t="s"/>
       <x:c r="J6" s="60" t="s"/>
     </x:row>
-    <x:row r="7" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="7" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A7" s="45" t="s"/>
       <x:c r="B7" s="61" t="s"/>
       <x:c r="C7" s="62" t="s"/>
@@ -1315,7 +1195,7 @@
       <x:c r="I7" s="45" t="s"/>
       <x:c r="J7" s="45" t="s"/>
     </x:row>
-    <x:row r="8" spans="1:10">
+    <x:row r="8" spans="1:11">
       <x:c r="A8" s="45" t="s"/>
       <x:c r="B8" s="50" t="s">
         <x:v>4</x:v>
@@ -1330,7 +1210,7 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="9" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A9" s="45" t="s"/>
       <x:c r="B9" s="63" t="s">
         <x:v>8</x:v>
@@ -1350,7 +1230,7 @@
       </x:c>
       <x:c r="J9" s="64" t="s"/>
     </x:row>
-    <x:row r="10" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="10" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A10" s="45" t="s"/>
       <x:c r="B10" s="65" t="s"/>
       <x:c r="C10" s="65" t="s"/>
@@ -1362,7 +1242,7 @@
       <x:c r="I10" s="65" t="s"/>
       <x:c r="J10" s="65" t="s"/>
     </x:row>
-    <x:row r="11" spans="1:10" customFormat="1" ht="22.5" customHeight="1">
+    <x:row r="11" spans="1:11" customFormat="1" ht="22.5" customHeight="1">
       <x:c r="A11" s="45" t="s"/>
       <x:c r="B11" s="66" t="s">
         <x:v>12</x:v>
@@ -1392,7 +1272,7 @@
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
+    <x:row r="12" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A12" s="45" t="s"/>
       <x:c r="B12" s="68" t="n">
         <x:v>1023</x:v>
@@ -1418,7 +1298,7 @@
         <x:v>4674</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
+    <x:row r="13" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A13" s="45" t="s"/>
       <x:c r="B13" s="68" t="n">
         <x:v>1123</x:v>
@@ -1444,7 +1324,7 @@
         <x:v>13945</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:10" customFormat="1" ht="12" customHeight="1" outlineLevel="1">
+    <x:row r="14" spans="1:11" customFormat="1" ht="12" customHeight="1" outlineLevel="1">
       <x:c r="A14" s="45" t="s"/>
       <x:c r="B14" s="74" t="s"/>
       <x:c r="C14" s="74" t="s"/>
@@ -1462,7 +1342,7 @@
         <x:f>Subtotal(9,J12:J13)</x:f>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
+    <x:row r="15" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A15" s="45" t="s"/>
       <x:c r="B15" s="68" t="n">
         <x:v>1269</x:v>
@@ -1488,7 +1368,7 @@
         <x:v>1400</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:10" customFormat="1" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1">
+    <x:row r="16" spans="1:11" customFormat="1" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1">
       <x:c r="A16" s="45" t="s"/>
       <x:c r="B16" s="68" t="n">
         <x:v>1169</x:v>
@@ -1514,7 +1394,7 @@
         <x:v>9471.95</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:10" outlineLevel="1">
+    <x:row r="17" spans="1:11" outlineLevel="1">
       <x:c r="A17" s="45" t="s"/>
       <x:c r="B17" s="74" t="s"/>
       <x:c r="C17" s="74" t="s"/>
@@ -1532,7 +1412,7 @@
         <x:f>Subtotal(9,J15:J16)</x:f>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
+    <x:row r="18" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A18" s="45" t="s"/>
       <x:c r="B18" s="68" t="n">
         <x:v>1176</x:v>
@@ -1558,7 +1438,7 @@
         <x:v>4178.85</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
+    <x:row r="19" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A19" s="45" t="s"/>
       <x:c r="B19" s="68" t="n">
         <x:v>1076</x:v>
@@ -1584,7 +1464,7 @@
         <x:v>17781</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:10" outlineLevel="1">
+    <x:row r="20" spans="1:11" outlineLevel="1">
       <x:c r="A20" s="45" t="s"/>
       <x:c r="B20" s="74" t="s"/>
       <x:c r="C20" s="74" t="s"/>
@@ -1602,7 +1482,7 @@
         <x:f>Subtotal(9,J18:J19)</x:f>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:10">
+    <x:row r="21" spans="1:11">
       <x:c r="A21" s="45" t="s"/>
       <x:c r="B21" s="74" t="s">
         <x:v>27</x:v>
@@ -1620,7 +1500,7 @@
         <x:f>Subtotal(9,J12:J19)</x:f>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:10">
+    <x:row r="22" spans="1:11">
       <x:c r="A22" s="45" t="s"/>
       <x:c r="B22" s="65" t="s"/>
       <x:c r="C22" s="65" t="s"/>
@@ -1632,7 +1512,7 @@
       <x:c r="I22" s="65" t="s"/>
       <x:c r="J22" s="65" t="s"/>
     </x:row>
-    <x:row r="23" spans="1:10">
+    <x:row r="23" spans="1:11">
       <x:c r="A23" s="45" t="s"/>
       <x:c r="B23" s="50" t="s">
         <x:v>28</x:v>
@@ -1641,7 +1521,7 @@
         <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:10">
+    <x:row r="24" spans="1:11">
       <x:c r="A24" s="45" t="s"/>
       <x:c r="B24" s="73" t="s">
         <x:v>30</x:v>
@@ -1657,17 +1537,17 @@
   </x:sheetData>
   <x:phoneticPr fontId="0" type="noConversion"/>
   <x:conditionalFormatting sqref="E18:G19">
-    <x:cfRule type="expression" dxfId="2" priority="1" operator="equal">
+    <x:cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <x:formula>$G18="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E15:G16">
-    <x:cfRule type="expression" dxfId="2" priority="2" operator="equal">
+    <x:cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <x:formula>$G15="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E12:G13">
-    <x:cfRule type="expression" dxfId="2" priority="3" operator="equal">
+    <x:cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
       <x:formula>$G12="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>

</xml_diff>

<commit_message>
Added output for tests
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Collapse.xlsx
+++ b/tests/Gauges/GroupTagTests_Collapse.xlsx
@@ -90,22 +90,22 @@
     <x:t>Check</x:t>
   </x:si>
   <x:si>
-    <x:t>Check Итог</x:t>
+    <x:t>Check Total</x:t>
   </x:si>
   <x:si>
     <x:t>Credit</x:t>
   </x:si>
   <x:si>
-    <x:t>Credit Итог</x:t>
+    <x:t>Credit Total</x:t>
   </x:si>
   <x:si>
     <x:t>Visa</x:t>
   </x:si>
   <x:si>
-    <x:t>Visa Итог</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Общий Итог</x:t>
+    <x:t>Visa Total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Общий Total</x:t>
   </x:si>
   <x:si>
     <x:t>Phone</x:t>

</xml_diff>

<commit_message>
- Added tag Delete - Added new tests - Added template validations - Improved based test class - Fixed bugs with grouping for nested groups - Fixed issues with Protect tag - Fixed issues with MergeLabels option for Group tag
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Collapse.xlsx
+++ b/tests/Gauges/GroupTagTests_Collapse.xlsx
@@ -10,7 +10,7 @@
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="Orders">Sheet1!$A$12:$J$21</x:definedName>
+    <x:definedName name="Orders">Sheet1!$A$12:$J$24</x:definedName>
     <x:definedName name="Orders_tpl">Sheet1!$A$12:$J$13</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <x:si>
     <x:t>Collapse outline</x:t>
   </x:si>
@@ -26,7 +26,7 @@
     <x:t>Customer</x:t>
   </x:si>
   <x:si>
-    <x:t>Kauai Dive Shoppe</x:t>
+    <x:t>Tom Sawyer Diving Centre</x:t>
   </x:si>
   <x:si>
     <x:t>Address</x:t>
@@ -44,16 +44,13 @@
     <x:t>Zip</x:t>
   </x:si>
   <x:si>
-    <x:t>Kapaa Kauai</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>US</x:t>
-  </x:si>
-  <x:si>
-    <x:t>94766-1234</x:t>
+    <x:t>Christiansted</x:t>
+  </x:si>
+  <x:si>
+    <x:t>St. Croix</x:t>
+  </x:si>
+  <x:si>
+    <x:t>US Virgin Islands</x:t>
   </x:si>
   <x:si>
     <x:t>Order No</x:t>
@@ -87,10 +84,16 @@
 paid</x:t>
   </x:si>
   <x:si>
-    <x:t>Check</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Check Total</x:t>
+    <x:t>Cash</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4-976 Sugarloaf Hwy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Suite 103</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cash Total</x:t>
   </x:si>
   <x:si>
     <x:t>Credit</x:t>
@@ -114,10 +117,10 @@
     <x:t>Fax</x:t>
   </x:si>
   <x:si>
-    <x:t>808-555-0269</x:t>
-  </x:si>
-  <x:si>
-    <x:t>808-555-0278</x:t>
+    <x:t>504-798-3022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>504-798-7772</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -588,12 +591,12 @@
       <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1105,10 +1108,9 @@
     <x:col min="8" max="8" width="9.164062" style="45" customWidth="1"/>
     <x:col min="9" max="9" width="7.332031" style="45" customWidth="1"/>
     <x:col min="10" max="10" width="11.5" style="45" customWidth="1"/>
-    <x:col min="11" max="11" width="9.140625" style="45" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:11" customFormat="1" ht="51" customHeight="1">
+    <x:row r="1" spans="1:10" customFormat="1" ht="51" customHeight="1">
       <x:c r="A1" s="45" t="s"/>
       <x:c r="B1" s="46" t="s">
         <x:v>0</x:v>
@@ -1122,7 +1124,7 @@
       <x:c r="I1" s="47" t="s"/>
       <x:c r="J1" s="47" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:11" customFormat="1" ht="12.75" customHeight="1">
+    <x:row r="2" spans="1:10" customFormat="1" ht="12.75" customHeight="1">
       <x:c r="A2" s="45" t="s"/>
       <x:c r="B2" s="48" t="s"/>
       <x:c r="C2" s="48" t="s"/>
@@ -1134,7 +1136,7 @@
       <x:c r="I2" s="48" t="s"/>
       <x:c r="J2" s="45" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:11" customFormat="1" ht="18" customHeight="1">
+    <x:row r="3" spans="1:10" customFormat="1" ht="18" customHeight="1">
       <x:c r="A3" s="49" t="s"/>
       <x:c r="B3" s="50" t="s">
         <x:v>1</x:v>
@@ -1150,7 +1152,7 @@
       <x:c r="I3" s="53" t="s"/>
       <x:c r="J3" s="54" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:11">
+    <x:row r="4" spans="1:10">
       <x:c r="A4" s="45" t="s"/>
       <x:c r="B4" s="55" t="s"/>
       <x:c r="C4" s="45" t="s"/>
@@ -1162,17 +1164,17 @@
       <x:c r="I4" s="45" t="s"/>
       <x:c r="J4" s="45" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:11">
+    <x:row r="5" spans="1:10">
       <x:c r="A5" s="45" t="s"/>
       <x:c r="B5" s="50" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C5" s="45" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:11" customFormat="1" ht="12" customHeight="1">
+    <x:row r="6" spans="1:10" customFormat="1" ht="12" customHeight="1">
       <x:c r="A6" s="45" t="s"/>
       <x:c r="B6" s="56" t="s">
-        <x:f>"4-976 Sugarloaf Hwy"&amp;" "&amp;"Suite 103"</x:f>
+        <x:f>"632-1 Third Frydenhoj"&amp;" "&amp;""</x:f>
       </x:c>
       <x:c r="C6" s="57" t="s"/>
       <x:c r="D6" s="57" t="s"/>
@@ -1183,7 +1185,7 @@
       <x:c r="I6" s="59" t="s"/>
       <x:c r="J6" s="60" t="s"/>
     </x:row>
-    <x:row r="7" spans="1:11" customFormat="1" ht="12" customHeight="1">
+    <x:row r="7" spans="1:10" customFormat="1" ht="12" customHeight="1">
       <x:c r="A7" s="45" t="s"/>
       <x:c r="B7" s="61" t="s"/>
       <x:c r="C7" s="62" t="s"/>
@@ -1195,7 +1197,7 @@
       <x:c r="I7" s="45" t="s"/>
       <x:c r="J7" s="45" t="s"/>
     </x:row>
-    <x:row r="8" spans="1:11">
+    <x:row r="8" spans="1:10">
       <x:c r="A8" s="45" t="s"/>
       <x:c r="B8" s="50" t="s">
         <x:v>4</x:v>
@@ -1210,7 +1212,7 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:11" customFormat="1" ht="12" customHeight="1">
+    <x:row r="9" spans="1:10" customFormat="1" ht="12" customHeight="1">
       <x:c r="A9" s="45" t="s"/>
       <x:c r="B9" s="63" t="s">
         <x:v>8</x:v>
@@ -1225,12 +1227,12 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="H9" s="64" t="s"/>
-      <x:c r="I9" s="63" t="s">
-        <x:v>11</x:v>
+      <x:c r="I9" s="63" t="n">
+        <x:v>820</x:v>
       </x:c>
       <x:c r="J9" s="64" t="s"/>
     </x:row>
-    <x:row r="10" spans="1:11" customFormat="1" ht="12" customHeight="1">
+    <x:row r="10" spans="1:10" customFormat="1" ht="12" customHeight="1">
       <x:c r="A10" s="45" t="s"/>
       <x:c r="B10" s="65" t="s"/>
       <x:c r="C10" s="65" t="s"/>
@@ -1242,89 +1244,93 @@
       <x:c r="I10" s="65" t="s"/>
       <x:c r="J10" s="65" t="s"/>
     </x:row>
-    <x:row r="11" spans="1:11" customFormat="1" ht="22.5" customHeight="1">
+    <x:row r="11" spans="1:10" customFormat="1" ht="22.5" customHeight="1">
       <x:c r="A11" s="45" t="s"/>
       <x:c r="B11" s="66" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C11" s="66" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C11" s="66" t="s">
+      <x:c r="D11" s="66" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D11" s="66" t="s">
+      <x:c r="E11" s="66" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E11" s="66" t="s">
+      <x:c r="F11" s="66" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="F11" s="66" t="s">
+      <x:c r="G11" s="67" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="G11" s="67" t="s">
+      <x:c r="H11" s="67" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="H11" s="67" t="s">
+      <x:c r="I11" s="67" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="I11" s="67" t="s">
+      <x:c r="J11" s="67" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="J11" s="67" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+    </x:row>
+    <x:row r="12" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A12" s="45" t="s"/>
       <x:c r="B12" s="68" t="n">
-        <x:v>1023</x:v>
+        <x:v>1072</x:v>
       </x:c>
       <x:c r="C12" s="69">
-        <x:v>32325</x:v>
+        <x:v>32609</x:v>
       </x:c>
       <x:c r="D12" s="69">
-        <x:v>32326</x:v>
+        <x:v>32610</x:v>
       </x:c>
       <x:c r="E12" s="70" t="s"/>
       <x:c r="F12" s="70" t="s"/>
       <x:c r="G12" s="70" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H12" s="71" t="n">
-        <x:v>4674</x:v>
+        <x:v>3596</x:v>
       </x:c>
       <x:c r="I12" s="71" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J12" s="71" t="n">
-        <x:v>4674</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+        <x:v>3596</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A13" s="45" t="s"/>
       <x:c r="B13" s="68" t="n">
-        <x:v>1123</x:v>
+        <x:v>1059</x:v>
       </x:c>
       <x:c r="C13" s="69">
-        <x:v>34205</x:v>
+        <x:v>32563</x:v>
       </x:c>
       <x:c r="D13" s="69">
-        <x:v>34205</x:v>
-      </x:c>
-      <x:c r="E13" s="70" t="s"/>
-      <x:c r="F13" s="70" t="s"/>
+        <x:v>32564</x:v>
+      </x:c>
+      <x:c r="E13" s="70" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F13" s="70" t="s">
+        <x:v>22</x:v>
+      </x:c>
       <x:c r="G13" s="70" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H13" s="71" t="n">
-        <x:v>13945</x:v>
+        <x:v>2150</x:v>
       </x:c>
       <x:c r="I13" s="71" t="n">
-        <x:v>0</x:v>
+        <x:v>8.5</x:v>
       </x:c>
       <x:c r="J13" s="71" t="n">
-        <x:v>13945</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:11" customFormat="1" ht="12" customHeight="1" outlineLevel="1">
+        <x:v>2150</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:10" customFormat="1" ht="12" customHeight="1" outlineLevel="1">
       <x:c r="A14" s="45" t="s"/>
       <x:c r="B14" s="74" t="s"/>
       <x:c r="C14" s="74" t="s"/>
@@ -1332,7 +1338,7 @@
       <x:c r="E14" s="74" t="s"/>
       <x:c r="F14" s="74" t="s"/>
       <x:c r="G14" s="75" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="H14" s="76" t="s"/>
       <x:c r="I14" s="74">
@@ -1342,213 +1348,292 @@
         <x:f>Subtotal(9,J12:J13)</x:f>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+    <x:row r="15" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A15" s="45" t="s"/>
       <x:c r="B15" s="68" t="n">
-        <x:v>1269</x:v>
+        <x:v>1280</x:v>
       </x:c>
       <x:c r="C15" s="69">
-        <x:v>34684</x:v>
+        <x:v>34694</x:v>
       </x:c>
       <x:c r="D15" s="69">
-        <x:v>34684</x:v>
+        <x:v>34694</x:v>
       </x:c>
       <x:c r="E15" s="70" t="s"/>
       <x:c r="F15" s="70" t="s"/>
       <x:c r="G15" s="70" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H15" s="71" t="n">
-        <x:v>1400</x:v>
+        <x:v>4317.75</x:v>
       </x:c>
       <x:c r="I15" s="71" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J15" s="71" t="n">
-        <x:v>1400</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:11" customFormat="1" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1">
+        <x:v>4317.75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:10" customFormat="1" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1">
       <x:c r="A16" s="45" t="s"/>
       <x:c r="B16" s="68" t="n">
-        <x:v>1169</x:v>
+        <x:v>1080</x:v>
       </x:c>
       <x:c r="C16" s="69">
-        <x:v>34521</x:v>
+        <x:v>32633</x:v>
       </x:c>
       <x:c r="D16" s="69">
-        <x:v>34521</x:v>
+        <x:v>32634</x:v>
       </x:c>
       <x:c r="E16" s="70" t="s"/>
       <x:c r="F16" s="70" t="s"/>
       <x:c r="G16" s="70" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H16" s="71" t="n">
-        <x:v>9471.95</x:v>
+        <x:v>9634</x:v>
       </x:c>
       <x:c r="I16" s="71" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J16" s="71" t="n">
-        <x:v>9471.95</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:11" outlineLevel="1">
+        <x:v>9634</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A17" s="45" t="s"/>
-      <x:c r="B17" s="74" t="s"/>
-      <x:c r="C17" s="74" t="s"/>
-      <x:c r="D17" s="74" t="s"/>
-      <x:c r="E17" s="74" t="s"/>
-      <x:c r="F17" s="74" t="s"/>
-      <x:c r="G17" s="75" t="s">
+      <x:c r="B17" s="68" t="n">
+        <x:v>1180</x:v>
+      </x:c>
+      <x:c r="C17" s="69">
+        <x:v>34552</x:v>
+      </x:c>
+      <x:c r="D17" s="69">
+        <x:v>34552</x:v>
+      </x:c>
+      <x:c r="E17" s="70" t="s"/>
+      <x:c r="F17" s="70" t="s"/>
+      <x:c r="G17" s="70" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="H17" s="76" t="s"/>
-      <x:c r="I17" s="74">
-        <x:f>Subtotal(9,I15:I16)</x:f>
-      </x:c>
-      <x:c r="J17" s="76">
-        <x:f>Subtotal(9,J15:J16)</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+      <x:c r="H17" s="71" t="n">
+        <x:v>3640</x:v>
+      </x:c>
+      <x:c r="I17" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J17" s="71" t="n">
+        <x:v>3640</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:10" outlineLevel="1">
       <x:c r="A18" s="45" t="s"/>
-      <x:c r="B18" s="68" t="n">
-        <x:v>1176</x:v>
-      </x:c>
-      <x:c r="C18" s="69">
-        <x:v>34541</x:v>
-      </x:c>
-      <x:c r="D18" s="69">
-        <x:v>34541</x:v>
-      </x:c>
-      <x:c r="E18" s="70" t="s"/>
-      <x:c r="F18" s="70" t="s"/>
-      <x:c r="G18" s="70" t="s">
+      <x:c r="B18" s="74" t="s"/>
+      <x:c r="C18" s="74" t="s"/>
+      <x:c r="D18" s="74" t="s"/>
+      <x:c r="E18" s="74" t="s"/>
+      <x:c r="F18" s="74" t="s"/>
+      <x:c r="G18" s="75" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H18" s="71" t="n">
-        <x:v>4178.85</x:v>
-      </x:c>
-      <x:c r="I18" s="71" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J18" s="71" t="n">
-        <x:v>4178.85</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+      <x:c r="H18" s="76" t="s"/>
+      <x:c r="I18" s="74">
+        <x:f>Subtotal(9,I15:I17)</x:f>
+      </x:c>
+      <x:c r="J18" s="76">
+        <x:f>Subtotal(9,J15:J17)</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A19" s="45" t="s"/>
       <x:c r="B19" s="68" t="n">
-        <x:v>1076</x:v>
+        <x:v>1105</x:v>
       </x:c>
       <x:c r="C19" s="69">
-        <x:v>34684</x:v>
+        <x:v>33806</x:v>
       </x:c>
       <x:c r="D19" s="69">
-        <x:v>32624</x:v>
+        <x:v>33806</x:v>
       </x:c>
       <x:c r="E19" s="70" t="s"/>
       <x:c r="F19" s="70" t="s"/>
       <x:c r="G19" s="70" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H19" s="71" t="n">
-        <x:v>17781</x:v>
+        <x:v>31219.95</x:v>
       </x:c>
       <x:c r="I19" s="71" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J19" s="71" t="n">
-        <x:v>17781</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:11" outlineLevel="1">
+        <x:v>31219.95</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A20" s="45" t="s"/>
-      <x:c r="B20" s="74" t="s"/>
-      <x:c r="C20" s="74" t="s"/>
-      <x:c r="D20" s="74" t="s"/>
-      <x:c r="E20" s="74" t="s"/>
-      <x:c r="F20" s="74" t="s"/>
-      <x:c r="G20" s="75" t="s">
+      <x:c r="B20" s="68" t="n">
+        <x:v>1266</x:v>
+      </x:c>
+      <x:c r="C20" s="69">
+        <x:v>34683</x:v>
+      </x:c>
+      <x:c r="D20" s="69">
+        <x:v>34683</x:v>
+      </x:c>
+      <x:c r="E20" s="70" t="s"/>
+      <x:c r="F20" s="70" t="s"/>
+      <x:c r="G20" s="70" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="H20" s="76" t="s"/>
-      <x:c r="I20" s="74">
-        <x:f>Subtotal(9,I18:I19)</x:f>
-      </x:c>
-      <x:c r="J20" s="76">
-        <x:f>Subtotal(9,J18:J19)</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:11">
+      <x:c r="H20" s="71" t="n">
+        <x:v>6935</x:v>
+      </x:c>
+      <x:c r="I20" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J20" s="71" t="n">
+        <x:v>6935</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A21" s="45" t="s"/>
-      <x:c r="B21" s="74" t="s">
+      <x:c r="B21" s="68" t="n">
+        <x:v>1005</x:v>
+      </x:c>
+      <x:c r="C21" s="69">
+        <x:v>32253</x:v>
+      </x:c>
+      <x:c r="D21" s="69">
+        <x:v>32163</x:v>
+      </x:c>
+      <x:c r="E21" s="70" t="s"/>
+      <x:c r="F21" s="70" t="s"/>
+      <x:c r="G21" s="70" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H21" s="71" t="n">
+        <x:v>4807</x:v>
+      </x:c>
+      <x:c r="I21" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J21" s="71" t="n">
+        <x:v>4807</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
+      <x:c r="A22" s="45" t="s"/>
+      <x:c r="B22" s="68" t="n">
+        <x:v>1305</x:v>
+      </x:c>
+      <x:c r="C22" s="69">
+        <x:v>34719</x:v>
+      </x:c>
+      <x:c r="D22" s="69">
+        <x:v>34719</x:v>
+      </x:c>
+      <x:c r="E22" s="70" t="s"/>
+      <x:c r="F22" s="70" t="s"/>
+      <x:c r="G22" s="70" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H22" s="71" t="n">
+        <x:v>3065</x:v>
+      </x:c>
+      <x:c r="I22" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J22" s="71" t="n">
+        <x:v>3065</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:10" outlineLevel="1">
+      <x:c r="A23" s="45" t="s"/>
+      <x:c r="B23" s="74" t="s"/>
+      <x:c r="C23" s="74" t="s"/>
+      <x:c r="D23" s="74" t="s"/>
+      <x:c r="E23" s="74" t="s"/>
+      <x:c r="F23" s="74" t="s"/>
+      <x:c r="G23" s="75" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C21" s="74" t="s"/>
-      <x:c r="D21" s="74" t="s"/>
-      <x:c r="E21" s="74" t="s"/>
-      <x:c r="F21" s="74" t="s"/>
-      <x:c r="G21" s="75" t="s"/>
-      <x:c r="H21" s="76" t="s"/>
-      <x:c r="I21" s="74">
-        <x:f>Subtotal(9,I12:I19)</x:f>
-      </x:c>
-      <x:c r="J21" s="76">
-        <x:f>Subtotal(9,J12:J19)</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:11">
-      <x:c r="A22" s="45" t="s"/>
-      <x:c r="B22" s="65" t="s"/>
-      <x:c r="C22" s="65" t="s"/>
-      <x:c r="D22" s="65" t="s"/>
-      <x:c r="E22" s="65" t="s"/>
-      <x:c r="F22" s="65" t="s"/>
-      <x:c r="G22" s="65" t="s"/>
-      <x:c r="H22" s="65" t="s"/>
-      <x:c r="I22" s="65" t="s"/>
-      <x:c r="J22" s="65" t="s"/>
-    </x:row>
-    <x:row r="23" spans="1:11">
-      <x:c r="A23" s="45" t="s"/>
-      <x:c r="B23" s="50" t="s">
+      <x:c r="H23" s="76" t="s"/>
+      <x:c r="I23" s="74">
+        <x:f>Subtotal(9,I19:I22)</x:f>
+      </x:c>
+      <x:c r="J23" s="76">
+        <x:f>Subtotal(9,J19:J22)</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:10">
+      <x:c r="A24" s="45" t="s"/>
+      <x:c r="B24" s="74" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="E23" s="50" t="s">
+      <x:c r="C24" s="74" t="s"/>
+      <x:c r="D24" s="74" t="s"/>
+      <x:c r="E24" s="74" t="s"/>
+      <x:c r="F24" s="74" t="s"/>
+      <x:c r="G24" s="75" t="s"/>
+      <x:c r="H24" s="76" t="s"/>
+      <x:c r="I24" s="74">
+        <x:f>Subtotal(9,I12:I22)</x:f>
+      </x:c>
+      <x:c r="J24" s="76">
+        <x:f>Subtotal(9,J12:J22)</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:10">
+      <x:c r="A25" s="45" t="s"/>
+      <x:c r="B25" s="65" t="s"/>
+      <x:c r="C25" s="65" t="s"/>
+      <x:c r="D25" s="65" t="s"/>
+      <x:c r="E25" s="65" t="s"/>
+      <x:c r="F25" s="65" t="s"/>
+      <x:c r="G25" s="65" t="s"/>
+      <x:c r="H25" s="65" t="s"/>
+      <x:c r="I25" s="65" t="s"/>
+      <x:c r="J25" s="65" t="s"/>
+    </x:row>
+    <x:row r="26" spans="1:10">
+      <x:c r="A26" s="45" t="s"/>
+      <x:c r="B26" s="50" t="s">
         <x:v>29</x:v>
       </x:c>
-    </x:row>
-    <x:row r="24" spans="1:11">
-      <x:c r="A24" s="45" t="s"/>
-      <x:c r="B24" s="73" t="s">
+      <x:c r="E26" s="50" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C24" s="57" t="s"/>
-      <x:c r="D24" s="57" t="s"/>
-      <x:c r="E24" s="73" t="s">
+    </x:row>
+    <x:row r="27" spans="1:10">
+      <x:c r="A27" s="45" t="s"/>
+      <x:c r="B27" s="72" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="F24" s="72" t="s"/>
-      <x:c r="G24" s="45" t="s"/>
+      <x:c r="C27" s="57" t="s"/>
+      <x:c r="D27" s="57" t="s"/>
+      <x:c r="E27" s="72" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F27" s="73" t="s"/>
+      <x:c r="G27" s="45" t="s"/>
+      <x:c r="J27" s="45" t="s"/>
     </x:row>
   </x:sheetData>
   <x:phoneticPr fontId="0" type="noConversion"/>
-  <x:conditionalFormatting sqref="E18:G19">
+  <x:conditionalFormatting sqref="E19:G22">
     <x:cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
-      <x:formula>$G18="Visa"</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E15:G16">
-    <x:cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
-      <x:formula>$G15="Visa"</x:formula>
+      <x:formula>$G19="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E12:G13">
+    <x:cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+      <x:formula>$G12="Visa"</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="E15:G17">
     <x:cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
-      <x:formula>$G12="Visa"</x:formula>
+      <x:formula>$G15="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
More bug fixes (#24)
* Some Facts converted to Theory

* - Added tag Delete
- Added new tests
- Added template validations
- Improved based test class
- Fixed bugs with grouping for nested groups
- Fixed issues with Protect tag
- Fixed issues with MergeLabels option for Group tag

* Cosmetic changes

* ColsFit tag fix

* changes for review requesting

* Added test ParseExceptionMessageShouldBeUnknownIdentifier

* Fix syntax error
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Collapse.xlsx
+++ b/tests/Gauges/GroupTagTests_Collapse.xlsx
@@ -10,7 +10,7 @@
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="Orders">Sheet1!$A$12:$J$21</x:definedName>
+    <x:definedName name="Orders">Sheet1!$A$12:$J$24</x:definedName>
     <x:definedName name="Orders_tpl">Sheet1!$A$12:$J$13</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <x:si>
     <x:t>Collapse outline</x:t>
   </x:si>
@@ -26,7 +26,7 @@
     <x:t>Customer</x:t>
   </x:si>
   <x:si>
-    <x:t>Kauai Dive Shoppe</x:t>
+    <x:t>Tom Sawyer Diving Centre</x:t>
   </x:si>
   <x:si>
     <x:t>Address</x:t>
@@ -44,16 +44,13 @@
     <x:t>Zip</x:t>
   </x:si>
   <x:si>
-    <x:t>Kapaa Kauai</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>US</x:t>
-  </x:si>
-  <x:si>
-    <x:t>94766-1234</x:t>
+    <x:t>Christiansted</x:t>
+  </x:si>
+  <x:si>
+    <x:t>St. Croix</x:t>
+  </x:si>
+  <x:si>
+    <x:t>US Virgin Islands</x:t>
   </x:si>
   <x:si>
     <x:t>Order No</x:t>
@@ -87,10 +84,16 @@
 paid</x:t>
   </x:si>
   <x:si>
-    <x:t>Check</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Check Total</x:t>
+    <x:t>Cash</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4-976 Sugarloaf Hwy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Suite 103</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cash Total</x:t>
   </x:si>
   <x:si>
     <x:t>Credit</x:t>
@@ -114,10 +117,10 @@
     <x:t>Fax</x:t>
   </x:si>
   <x:si>
-    <x:t>808-555-0269</x:t>
-  </x:si>
-  <x:si>
-    <x:t>808-555-0278</x:t>
+    <x:t>504-798-3022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>504-798-7772</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -588,12 +591,12 @@
       <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1105,10 +1108,9 @@
     <x:col min="8" max="8" width="9.164062" style="45" customWidth="1"/>
     <x:col min="9" max="9" width="7.332031" style="45" customWidth="1"/>
     <x:col min="10" max="10" width="11.5" style="45" customWidth="1"/>
-    <x:col min="11" max="11" width="9.140625" style="45" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:11" customFormat="1" ht="51" customHeight="1">
+    <x:row r="1" spans="1:10" customFormat="1" ht="51" customHeight="1">
       <x:c r="A1" s="45" t="s"/>
       <x:c r="B1" s="46" t="s">
         <x:v>0</x:v>
@@ -1122,7 +1124,7 @@
       <x:c r="I1" s="47" t="s"/>
       <x:c r="J1" s="47" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:11" customFormat="1" ht="12.75" customHeight="1">
+    <x:row r="2" spans="1:10" customFormat="1" ht="12.75" customHeight="1">
       <x:c r="A2" s="45" t="s"/>
       <x:c r="B2" s="48" t="s"/>
       <x:c r="C2" s="48" t="s"/>
@@ -1134,7 +1136,7 @@
       <x:c r="I2" s="48" t="s"/>
       <x:c r="J2" s="45" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:11" customFormat="1" ht="18" customHeight="1">
+    <x:row r="3" spans="1:10" customFormat="1" ht="18" customHeight="1">
       <x:c r="A3" s="49" t="s"/>
       <x:c r="B3" s="50" t="s">
         <x:v>1</x:v>
@@ -1150,7 +1152,7 @@
       <x:c r="I3" s="53" t="s"/>
       <x:c r="J3" s="54" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:11">
+    <x:row r="4" spans="1:10">
       <x:c r="A4" s="45" t="s"/>
       <x:c r="B4" s="55" t="s"/>
       <x:c r="C4" s="45" t="s"/>
@@ -1162,17 +1164,17 @@
       <x:c r="I4" s="45" t="s"/>
       <x:c r="J4" s="45" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:11">
+    <x:row r="5" spans="1:10">
       <x:c r="A5" s="45" t="s"/>
       <x:c r="B5" s="50" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C5" s="45" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:11" customFormat="1" ht="12" customHeight="1">
+    <x:row r="6" spans="1:10" customFormat="1" ht="12" customHeight="1">
       <x:c r="A6" s="45" t="s"/>
       <x:c r="B6" s="56" t="s">
-        <x:f>"4-976 Sugarloaf Hwy"&amp;" "&amp;"Suite 103"</x:f>
+        <x:f>"632-1 Third Frydenhoj"&amp;" "&amp;""</x:f>
       </x:c>
       <x:c r="C6" s="57" t="s"/>
       <x:c r="D6" s="57" t="s"/>
@@ -1183,7 +1185,7 @@
       <x:c r="I6" s="59" t="s"/>
       <x:c r="J6" s="60" t="s"/>
     </x:row>
-    <x:row r="7" spans="1:11" customFormat="1" ht="12" customHeight="1">
+    <x:row r="7" spans="1:10" customFormat="1" ht="12" customHeight="1">
       <x:c r="A7" s="45" t="s"/>
       <x:c r="B7" s="61" t="s"/>
       <x:c r="C7" s="62" t="s"/>
@@ -1195,7 +1197,7 @@
       <x:c r="I7" s="45" t="s"/>
       <x:c r="J7" s="45" t="s"/>
     </x:row>
-    <x:row r="8" spans="1:11">
+    <x:row r="8" spans="1:10">
       <x:c r="A8" s="45" t="s"/>
       <x:c r="B8" s="50" t="s">
         <x:v>4</x:v>
@@ -1210,7 +1212,7 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:11" customFormat="1" ht="12" customHeight="1">
+    <x:row r="9" spans="1:10" customFormat="1" ht="12" customHeight="1">
       <x:c r="A9" s="45" t="s"/>
       <x:c r="B9" s="63" t="s">
         <x:v>8</x:v>
@@ -1225,12 +1227,12 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="H9" s="64" t="s"/>
-      <x:c r="I9" s="63" t="s">
-        <x:v>11</x:v>
+      <x:c r="I9" s="63" t="n">
+        <x:v>820</x:v>
       </x:c>
       <x:c r="J9" s="64" t="s"/>
     </x:row>
-    <x:row r="10" spans="1:11" customFormat="1" ht="12" customHeight="1">
+    <x:row r="10" spans="1:10" customFormat="1" ht="12" customHeight="1">
       <x:c r="A10" s="45" t="s"/>
       <x:c r="B10" s="65" t="s"/>
       <x:c r="C10" s="65" t="s"/>
@@ -1242,89 +1244,93 @@
       <x:c r="I10" s="65" t="s"/>
       <x:c r="J10" s="65" t="s"/>
     </x:row>
-    <x:row r="11" spans="1:11" customFormat="1" ht="22.5" customHeight="1">
+    <x:row r="11" spans="1:10" customFormat="1" ht="22.5" customHeight="1">
       <x:c r="A11" s="45" t="s"/>
       <x:c r="B11" s="66" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C11" s="66" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C11" s="66" t="s">
+      <x:c r="D11" s="66" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D11" s="66" t="s">
+      <x:c r="E11" s="66" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E11" s="66" t="s">
+      <x:c r="F11" s="66" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="F11" s="66" t="s">
+      <x:c r="G11" s="67" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="G11" s="67" t="s">
+      <x:c r="H11" s="67" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="H11" s="67" t="s">
+      <x:c r="I11" s="67" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="I11" s="67" t="s">
+      <x:c r="J11" s="67" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="J11" s="67" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+    </x:row>
+    <x:row r="12" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A12" s="45" t="s"/>
       <x:c r="B12" s="68" t="n">
-        <x:v>1023</x:v>
+        <x:v>1072</x:v>
       </x:c>
       <x:c r="C12" s="69">
-        <x:v>32325</x:v>
+        <x:v>32609</x:v>
       </x:c>
       <x:c r="D12" s="69">
-        <x:v>32326</x:v>
+        <x:v>32610</x:v>
       </x:c>
       <x:c r="E12" s="70" t="s"/>
       <x:c r="F12" s="70" t="s"/>
       <x:c r="G12" s="70" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H12" s="71" t="n">
-        <x:v>4674</x:v>
+        <x:v>3596</x:v>
       </x:c>
       <x:c r="I12" s="71" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J12" s="71" t="n">
-        <x:v>4674</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+        <x:v>3596</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A13" s="45" t="s"/>
       <x:c r="B13" s="68" t="n">
-        <x:v>1123</x:v>
+        <x:v>1059</x:v>
       </x:c>
       <x:c r="C13" s="69">
-        <x:v>34205</x:v>
+        <x:v>32563</x:v>
       </x:c>
       <x:c r="D13" s="69">
-        <x:v>34205</x:v>
-      </x:c>
-      <x:c r="E13" s="70" t="s"/>
-      <x:c r="F13" s="70" t="s"/>
+        <x:v>32564</x:v>
+      </x:c>
+      <x:c r="E13" s="70" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F13" s="70" t="s">
+        <x:v>22</x:v>
+      </x:c>
       <x:c r="G13" s="70" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H13" s="71" t="n">
-        <x:v>13945</x:v>
+        <x:v>2150</x:v>
       </x:c>
       <x:c r="I13" s="71" t="n">
-        <x:v>0</x:v>
+        <x:v>8.5</x:v>
       </x:c>
       <x:c r="J13" s="71" t="n">
-        <x:v>13945</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:11" customFormat="1" ht="12" customHeight="1" outlineLevel="1">
+        <x:v>2150</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:10" customFormat="1" ht="12" customHeight="1" outlineLevel="1">
       <x:c r="A14" s="45" t="s"/>
       <x:c r="B14" s="74" t="s"/>
       <x:c r="C14" s="74" t="s"/>
@@ -1332,7 +1338,7 @@
       <x:c r="E14" s="74" t="s"/>
       <x:c r="F14" s="74" t="s"/>
       <x:c r="G14" s="75" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="H14" s="76" t="s"/>
       <x:c r="I14" s="74">
@@ -1342,213 +1348,292 @@
         <x:f>Subtotal(9,J12:J13)</x:f>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+    <x:row r="15" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A15" s="45" t="s"/>
       <x:c r="B15" s="68" t="n">
-        <x:v>1269</x:v>
+        <x:v>1280</x:v>
       </x:c>
       <x:c r="C15" s="69">
-        <x:v>34684</x:v>
+        <x:v>34694</x:v>
       </x:c>
       <x:c r="D15" s="69">
-        <x:v>34684</x:v>
+        <x:v>34694</x:v>
       </x:c>
       <x:c r="E15" s="70" t="s"/>
       <x:c r="F15" s="70" t="s"/>
       <x:c r="G15" s="70" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H15" s="71" t="n">
-        <x:v>1400</x:v>
+        <x:v>4317.75</x:v>
       </x:c>
       <x:c r="I15" s="71" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J15" s="71" t="n">
-        <x:v>1400</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:11" customFormat="1" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1">
+        <x:v>4317.75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:10" customFormat="1" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1">
       <x:c r="A16" s="45" t="s"/>
       <x:c r="B16" s="68" t="n">
-        <x:v>1169</x:v>
+        <x:v>1080</x:v>
       </x:c>
       <x:c r="C16" s="69">
-        <x:v>34521</x:v>
+        <x:v>32633</x:v>
       </x:c>
       <x:c r="D16" s="69">
-        <x:v>34521</x:v>
+        <x:v>32634</x:v>
       </x:c>
       <x:c r="E16" s="70" t="s"/>
       <x:c r="F16" s="70" t="s"/>
       <x:c r="G16" s="70" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H16" s="71" t="n">
-        <x:v>9471.95</x:v>
+        <x:v>9634</x:v>
       </x:c>
       <x:c r="I16" s="71" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J16" s="71" t="n">
-        <x:v>9471.95</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:11" outlineLevel="1">
+        <x:v>9634</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A17" s="45" t="s"/>
-      <x:c r="B17" s="74" t="s"/>
-      <x:c r="C17" s="74" t="s"/>
-      <x:c r="D17" s="74" t="s"/>
-      <x:c r="E17" s="74" t="s"/>
-      <x:c r="F17" s="74" t="s"/>
-      <x:c r="G17" s="75" t="s">
+      <x:c r="B17" s="68" t="n">
+        <x:v>1180</x:v>
+      </x:c>
+      <x:c r="C17" s="69">
+        <x:v>34552</x:v>
+      </x:c>
+      <x:c r="D17" s="69">
+        <x:v>34552</x:v>
+      </x:c>
+      <x:c r="E17" s="70" t="s"/>
+      <x:c r="F17" s="70" t="s"/>
+      <x:c r="G17" s="70" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="H17" s="76" t="s"/>
-      <x:c r="I17" s="74">
-        <x:f>Subtotal(9,I15:I16)</x:f>
-      </x:c>
-      <x:c r="J17" s="76">
-        <x:f>Subtotal(9,J15:J16)</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+      <x:c r="H17" s="71" t="n">
+        <x:v>3640</x:v>
+      </x:c>
+      <x:c r="I17" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J17" s="71" t="n">
+        <x:v>3640</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:10" outlineLevel="1">
       <x:c r="A18" s="45" t="s"/>
-      <x:c r="B18" s="68" t="n">
-        <x:v>1176</x:v>
-      </x:c>
-      <x:c r="C18" s="69">
-        <x:v>34541</x:v>
-      </x:c>
-      <x:c r="D18" s="69">
-        <x:v>34541</x:v>
-      </x:c>
-      <x:c r="E18" s="70" t="s"/>
-      <x:c r="F18" s="70" t="s"/>
-      <x:c r="G18" s="70" t="s">
+      <x:c r="B18" s="74" t="s"/>
+      <x:c r="C18" s="74" t="s"/>
+      <x:c r="D18" s="74" t="s"/>
+      <x:c r="E18" s="74" t="s"/>
+      <x:c r="F18" s="74" t="s"/>
+      <x:c r="G18" s="75" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H18" s="71" t="n">
-        <x:v>4178.85</x:v>
-      </x:c>
-      <x:c r="I18" s="71" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J18" s="71" t="n">
-        <x:v>4178.85</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:11" hidden="1" outlineLevel="2" collapsed="1">
+      <x:c r="H18" s="76" t="s"/>
+      <x:c r="I18" s="74">
+        <x:f>Subtotal(9,I15:I17)</x:f>
+      </x:c>
+      <x:c r="J18" s="76">
+        <x:f>Subtotal(9,J15:J17)</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A19" s="45" t="s"/>
       <x:c r="B19" s="68" t="n">
-        <x:v>1076</x:v>
+        <x:v>1105</x:v>
       </x:c>
       <x:c r="C19" s="69">
-        <x:v>34684</x:v>
+        <x:v>33806</x:v>
       </x:c>
       <x:c r="D19" s="69">
-        <x:v>32624</x:v>
+        <x:v>33806</x:v>
       </x:c>
       <x:c r="E19" s="70" t="s"/>
       <x:c r="F19" s="70" t="s"/>
       <x:c r="G19" s="70" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H19" s="71" t="n">
-        <x:v>17781</x:v>
+        <x:v>31219.95</x:v>
       </x:c>
       <x:c r="I19" s="71" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J19" s="71" t="n">
-        <x:v>17781</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:11" outlineLevel="1">
+        <x:v>31219.95</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A20" s="45" t="s"/>
-      <x:c r="B20" s="74" t="s"/>
-      <x:c r="C20" s="74" t="s"/>
-      <x:c r="D20" s="74" t="s"/>
-      <x:c r="E20" s="74" t="s"/>
-      <x:c r="F20" s="74" t="s"/>
-      <x:c r="G20" s="75" t="s">
+      <x:c r="B20" s="68" t="n">
+        <x:v>1266</x:v>
+      </x:c>
+      <x:c r="C20" s="69">
+        <x:v>34683</x:v>
+      </x:c>
+      <x:c r="D20" s="69">
+        <x:v>34683</x:v>
+      </x:c>
+      <x:c r="E20" s="70" t="s"/>
+      <x:c r="F20" s="70" t="s"/>
+      <x:c r="G20" s="70" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="H20" s="76" t="s"/>
-      <x:c r="I20" s="74">
-        <x:f>Subtotal(9,I18:I19)</x:f>
-      </x:c>
-      <x:c r="J20" s="76">
-        <x:f>Subtotal(9,J18:J19)</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:11">
+      <x:c r="H20" s="71" t="n">
+        <x:v>6935</x:v>
+      </x:c>
+      <x:c r="I20" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J20" s="71" t="n">
+        <x:v>6935</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
       <x:c r="A21" s="45" t="s"/>
-      <x:c r="B21" s="74" t="s">
+      <x:c r="B21" s="68" t="n">
+        <x:v>1005</x:v>
+      </x:c>
+      <x:c r="C21" s="69">
+        <x:v>32253</x:v>
+      </x:c>
+      <x:c r="D21" s="69">
+        <x:v>32163</x:v>
+      </x:c>
+      <x:c r="E21" s="70" t="s"/>
+      <x:c r="F21" s="70" t="s"/>
+      <x:c r="G21" s="70" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H21" s="71" t="n">
+        <x:v>4807</x:v>
+      </x:c>
+      <x:c r="I21" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J21" s="71" t="n">
+        <x:v>4807</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
+      <x:c r="A22" s="45" t="s"/>
+      <x:c r="B22" s="68" t="n">
+        <x:v>1305</x:v>
+      </x:c>
+      <x:c r="C22" s="69">
+        <x:v>34719</x:v>
+      </x:c>
+      <x:c r="D22" s="69">
+        <x:v>34719</x:v>
+      </x:c>
+      <x:c r="E22" s="70" t="s"/>
+      <x:c r="F22" s="70" t="s"/>
+      <x:c r="G22" s="70" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H22" s="71" t="n">
+        <x:v>3065</x:v>
+      </x:c>
+      <x:c r="I22" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J22" s="71" t="n">
+        <x:v>3065</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:10" outlineLevel="1">
+      <x:c r="A23" s="45" t="s"/>
+      <x:c r="B23" s="74" t="s"/>
+      <x:c r="C23" s="74" t="s"/>
+      <x:c r="D23" s="74" t="s"/>
+      <x:c r="E23" s="74" t="s"/>
+      <x:c r="F23" s="74" t="s"/>
+      <x:c r="G23" s="75" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C21" s="74" t="s"/>
-      <x:c r="D21" s="74" t="s"/>
-      <x:c r="E21" s="74" t="s"/>
-      <x:c r="F21" s="74" t="s"/>
-      <x:c r="G21" s="75" t="s"/>
-      <x:c r="H21" s="76" t="s"/>
-      <x:c r="I21" s="74">
-        <x:f>Subtotal(9,I12:I19)</x:f>
-      </x:c>
-      <x:c r="J21" s="76">
-        <x:f>Subtotal(9,J12:J19)</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:11">
-      <x:c r="A22" s="45" t="s"/>
-      <x:c r="B22" s="65" t="s"/>
-      <x:c r="C22" s="65" t="s"/>
-      <x:c r="D22" s="65" t="s"/>
-      <x:c r="E22" s="65" t="s"/>
-      <x:c r="F22" s="65" t="s"/>
-      <x:c r="G22" s="65" t="s"/>
-      <x:c r="H22" s="65" t="s"/>
-      <x:c r="I22" s="65" t="s"/>
-      <x:c r="J22" s="65" t="s"/>
-    </x:row>
-    <x:row r="23" spans="1:11">
-      <x:c r="A23" s="45" t="s"/>
-      <x:c r="B23" s="50" t="s">
+      <x:c r="H23" s="76" t="s"/>
+      <x:c r="I23" s="74">
+        <x:f>Subtotal(9,I19:I22)</x:f>
+      </x:c>
+      <x:c r="J23" s="76">
+        <x:f>Subtotal(9,J19:J22)</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:10">
+      <x:c r="A24" s="45" t="s"/>
+      <x:c r="B24" s="74" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="E23" s="50" t="s">
+      <x:c r="C24" s="74" t="s"/>
+      <x:c r="D24" s="74" t="s"/>
+      <x:c r="E24" s="74" t="s"/>
+      <x:c r="F24" s="74" t="s"/>
+      <x:c r="G24" s="75" t="s"/>
+      <x:c r="H24" s="76" t="s"/>
+      <x:c r="I24" s="74">
+        <x:f>Subtotal(9,I12:I22)</x:f>
+      </x:c>
+      <x:c r="J24" s="76">
+        <x:f>Subtotal(9,J12:J22)</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:10">
+      <x:c r="A25" s="45" t="s"/>
+      <x:c r="B25" s="65" t="s"/>
+      <x:c r="C25" s="65" t="s"/>
+      <x:c r="D25" s="65" t="s"/>
+      <x:c r="E25" s="65" t="s"/>
+      <x:c r="F25" s="65" t="s"/>
+      <x:c r="G25" s="65" t="s"/>
+      <x:c r="H25" s="65" t="s"/>
+      <x:c r="I25" s="65" t="s"/>
+      <x:c r="J25" s="65" t="s"/>
+    </x:row>
+    <x:row r="26" spans="1:10">
+      <x:c r="A26" s="45" t="s"/>
+      <x:c r="B26" s="50" t="s">
         <x:v>29</x:v>
       </x:c>
-    </x:row>
-    <x:row r="24" spans="1:11">
-      <x:c r="A24" s="45" t="s"/>
-      <x:c r="B24" s="73" t="s">
+      <x:c r="E26" s="50" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C24" s="57" t="s"/>
-      <x:c r="D24" s="57" t="s"/>
-      <x:c r="E24" s="73" t="s">
+    </x:row>
+    <x:row r="27" spans="1:10">
+      <x:c r="A27" s="45" t="s"/>
+      <x:c r="B27" s="72" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="F24" s="72" t="s"/>
-      <x:c r="G24" s="45" t="s"/>
+      <x:c r="C27" s="57" t="s"/>
+      <x:c r="D27" s="57" t="s"/>
+      <x:c r="E27" s="72" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F27" s="73" t="s"/>
+      <x:c r="G27" s="45" t="s"/>
+      <x:c r="J27" s="45" t="s"/>
     </x:row>
   </x:sheetData>
   <x:phoneticPr fontId="0" type="noConversion"/>
-  <x:conditionalFormatting sqref="E18:G19">
+  <x:conditionalFormatting sqref="E19:G22">
     <x:cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
-      <x:formula>$G18="Visa"</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E15:G16">
-    <x:cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
-      <x:formula>$G15="Visa"</x:formula>
+      <x:formula>$G19="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:conditionalFormatting sqref="E12:G13">
+    <x:cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+      <x:formula>$G12="Visa"</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:conditionalFormatting sqref="E15:G17">
     <x:cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
-      <x:formula>$G12="Visa"</x:formula>
+      <x:formula>$G15="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Upgrade a reference file: consolidate conditional formats and other minor changes
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Collapse.xlsx
+++ b/tests/Gauges/GroupTagTests_Collapse.xlsx
@@ -309,11 +309,8 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="23">
+  <x:cellStyleXfs count="22">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -368,17 +365,17 @@
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="77">
+  <x:cellXfs count="67">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -486,10 +483,6 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <x:xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -510,46 +503,14 @@
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -558,10 +519,6 @@
       <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -594,24 +551,24 @@
       <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -621,10 +578,6 @@
   <x:dxfs count="1">
     <x:dxf>
       <x:font>
-        <x:b val="0"/>
-        <x:i val="0"/>
-        <x:condense val="0"/>
-        <x:extend val="0"/>
         <x:color indexed="30"/>
       </x:font>
     </x:dxf>
@@ -711,9 +664,9 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1695450" cy="609600"/>
+    <xdr:ext cx="1699260" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Рисунок 2"/>
@@ -730,7 +683,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1695450" cy="609600"/>
+          <a:ext cx="1699260" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
       </xdr:spPr>
@@ -1101,542 +1054,492 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="2"/>
   <x:cols>
-    <x:col min="1" max="1" width="2.832031" style="45" customWidth="1"/>
-    <x:col min="2" max="2" width="9" style="45" customWidth="1"/>
-    <x:col min="3" max="3" width="9.664062" style="45" customWidth="1"/>
-    <x:col min="4" max="4" width="9.140625" style="45" customWidth="1"/>
-    <x:col min="5" max="5" width="6.164062" style="45" customWidth="1"/>
-    <x:col min="6" max="6" width="6.832031" style="45" customWidth="1"/>
-    <x:col min="7" max="7" width="8.5" style="45" customWidth="1"/>
-    <x:col min="8" max="8" width="9.164062" style="45" customWidth="1"/>
-    <x:col min="9" max="9" width="7.332031" style="45" customWidth="1"/>
-    <x:col min="10" max="10" width="11.5" style="45" customWidth="1"/>
+    <x:col min="1" max="1" width="2.832031" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="9" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="9.664062" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="6.164062" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="6.832031" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="8.5" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="9.164062" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="7.332031" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="11.5" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:10" customFormat="1" ht="51" customHeight="1">
-      <x:c r="A1" s="45" t="s"/>
-      <x:c r="B1" s="46" t="s">
+      <x:c r="B1" s="45" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C1" s="47" t="s"/>
-      <x:c r="D1" s="47" t="s"/>
-      <x:c r="E1" s="47" t="s"/>
-      <x:c r="F1" s="47" t="s"/>
-      <x:c r="G1" s="47" t="s"/>
-      <x:c r="H1" s="47" t="s"/>
-      <x:c r="I1" s="47" t="s"/>
-      <x:c r="J1" s="47" t="s"/>
+      <x:c r="C1" s="46" t="s"/>
+      <x:c r="D1" s="46" t="s"/>
+      <x:c r="E1" s="46" t="s"/>
+      <x:c r="F1" s="46" t="s"/>
+      <x:c r="G1" s="46" t="s"/>
+      <x:c r="H1" s="46" t="s"/>
+      <x:c r="I1" s="46" t="s"/>
+      <x:c r="J1" s="46" t="s"/>
     </x:row>
     <x:row r="2" spans="1:10" customFormat="1" ht="12.75" customHeight="1">
-      <x:c r="A2" s="45" t="s"/>
-      <x:c r="B2" s="48" t="s"/>
-      <x:c r="C2" s="48" t="s"/>
-      <x:c r="D2" s="48" t="s"/>
-      <x:c r="E2" s="48" t="s"/>
-      <x:c r="F2" s="48" t="s"/>
-      <x:c r="G2" s="48" t="s"/>
-      <x:c r="H2" s="48" t="s"/>
-      <x:c r="I2" s="48" t="s"/>
-      <x:c r="J2" s="45" t="s"/>
+      <x:c r="B2" s="47" t="s"/>
+      <x:c r="C2" s="47" t="s"/>
+      <x:c r="D2" s="47" t="s"/>
+      <x:c r="E2" s="47" t="s"/>
+      <x:c r="F2" s="47" t="s"/>
+      <x:c r="G2" s="47" t="s"/>
+      <x:c r="H2" s="47" t="s"/>
+      <x:c r="I2" s="47" t="s"/>
     </x:row>
     <x:row r="3" spans="1:10" customFormat="1" ht="18" customHeight="1">
-      <x:c r="A3" s="49" t="s"/>
-      <x:c r="B3" s="50" t="s">
+      <x:c r="A3" s="48" t="s"/>
+      <x:c r="B3" s="49" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="51" t="s">
+      <x:c r="C3" s="32" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D3" s="52" t="s"/>
-      <x:c r="E3" s="52" t="s"/>
-      <x:c r="F3" s="52" t="s"/>
-      <x:c r="G3" s="53" t="s"/>
-      <x:c r="H3" s="53" t="s"/>
-      <x:c r="I3" s="53" t="s"/>
-      <x:c r="J3" s="54" t="s"/>
+      <x:c r="D3" s="21" t="s"/>
+      <x:c r="E3" s="21" t="s"/>
+      <x:c r="F3" s="21" t="s"/>
+      <x:c r="G3" s="17" t="s"/>
+      <x:c r="H3" s="17" t="s"/>
+      <x:c r="I3" s="17" t="s"/>
+      <x:c r="J3" s="18" t="s"/>
     </x:row>
     <x:row r="4" spans="1:10">
-      <x:c r="A4" s="45" t="s"/>
-      <x:c r="B4" s="55" t="s"/>
-      <x:c r="C4" s="45" t="s"/>
-      <x:c r="D4" s="45" t="s"/>
-      <x:c r="E4" s="45" t="s"/>
-      <x:c r="F4" s="45" t="s"/>
-      <x:c r="G4" s="45" t="s"/>
-      <x:c r="H4" s="45" t="s"/>
-      <x:c r="I4" s="45" t="s"/>
-      <x:c r="J4" s="45" t="s"/>
+      <x:c r="B4" s="50" t="s"/>
     </x:row>
     <x:row r="5" spans="1:10">
-      <x:c r="A5" s="45" t="s"/>
-      <x:c r="B5" s="50" t="s">
+      <x:c r="B5" s="49" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C5" s="45" t="s"/>
     </x:row>
     <x:row r="6" spans="1:10" customFormat="1" ht="12" customHeight="1">
-      <x:c r="A6" s="45" t="s"/>
-      <x:c r="B6" s="56" t="s">
+      <x:c r="B6" s="42" t="s">
         <x:f>"632-1 Third Frydenhoj"&amp;" "&amp;""</x:f>
       </x:c>
-      <x:c r="C6" s="57" t="s"/>
-      <x:c r="D6" s="57" t="s"/>
-      <x:c r="E6" s="57" t="s"/>
-      <x:c r="F6" s="57" t="s"/>
-      <x:c r="G6" s="57" t="s"/>
-      <x:c r="H6" s="58" t="s"/>
-      <x:c r="I6" s="59" t="s"/>
-      <x:c r="J6" s="60" t="s"/>
+      <x:c r="C6" s="13" t="s"/>
+      <x:c r="D6" s="13" t="s"/>
+      <x:c r="E6" s="13" t="s"/>
+      <x:c r="F6" s="13" t="s"/>
+      <x:c r="G6" s="13" t="s"/>
+      <x:c r="H6" s="51" t="s"/>
+      <x:c r="I6" s="15" t="s"/>
+      <x:c r="J6" s="16" t="s"/>
     </x:row>
     <x:row r="7" spans="1:10" customFormat="1" ht="12" customHeight="1">
-      <x:c r="A7" s="45" t="s"/>
-      <x:c r="B7" s="61" t="s"/>
-      <x:c r="C7" s="62" t="s"/>
-      <x:c r="D7" s="62" t="s"/>
-      <x:c r="E7" s="62" t="s"/>
-      <x:c r="F7" s="62" t="s"/>
-      <x:c r="G7" s="62" t="s"/>
-      <x:c r="H7" s="61" t="s"/>
-      <x:c r="I7" s="45" t="s"/>
-      <x:c r="J7" s="45" t="s"/>
+      <x:c r="B7" s="52" t="s"/>
+      <x:c r="C7" s="53" t="s"/>
+      <x:c r="D7" s="53" t="s"/>
+      <x:c r="E7" s="53" t="s"/>
+      <x:c r="F7" s="53" t="s"/>
+      <x:c r="G7" s="53" t="s"/>
+      <x:c r="H7" s="52" t="s"/>
     </x:row>
     <x:row r="8" spans="1:10">
-      <x:c r="A8" s="45" t="s"/>
-      <x:c r="B8" s="50" t="s">
+      <x:c r="B8" s="49" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="E8" s="50" t="s">
+      <x:c r="E8" s="49" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G8" s="50" t="s">
+      <x:c r="G8" s="49" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="I8" s="50" t="s">
+      <x:c r="I8" s="49" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10" customFormat="1" ht="12" customHeight="1">
-      <x:c r="A9" s="45" t="s"/>
-      <x:c r="B9" s="63" t="s">
+      <x:c r="B9" s="35" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C9" s="57" t="s"/>
-      <x:c r="D9" s="57" t="s"/>
-      <x:c r="E9" s="63" t="s">
+      <x:c r="C9" s="13" t="s"/>
+      <x:c r="D9" s="13" t="s"/>
+      <x:c r="E9" s="35" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F9" s="64" t="s"/>
-      <x:c r="G9" s="63" t="s">
+      <x:c r="F9" s="54" t="s"/>
+      <x:c r="G9" s="35" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="H9" s="64" t="s"/>
-      <x:c r="I9" s="63" t="s">
+      <x:c r="H9" s="54" t="s"/>
+      <x:c r="I9" s="35" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="J9" s="64" t="s"/>
+      <x:c r="J9" s="54" t="s"/>
     </x:row>
     <x:row r="10" spans="1:10" customFormat="1" ht="12" customHeight="1">
-      <x:c r="A10" s="45" t="s"/>
-      <x:c r="B10" s="65" t="s"/>
-      <x:c r="C10" s="65" t="s"/>
-      <x:c r="D10" s="65" t="s"/>
-      <x:c r="E10" s="65" t="s"/>
-      <x:c r="F10" s="65" t="s"/>
-      <x:c r="G10" s="65" t="s"/>
-      <x:c r="H10" s="65" t="s"/>
-      <x:c r="I10" s="65" t="s"/>
-      <x:c r="J10" s="65" t="s"/>
+      <x:c r="B10" s="55" t="s"/>
+      <x:c r="C10" s="55" t="s"/>
+      <x:c r="D10" s="55" t="s"/>
+      <x:c r="E10" s="55" t="s"/>
+      <x:c r="F10" s="55" t="s"/>
+      <x:c r="G10" s="55" t="s"/>
+      <x:c r="H10" s="55" t="s"/>
+      <x:c r="I10" s="55" t="s"/>
+      <x:c r="J10" s="55" t="s"/>
     </x:row>
     <x:row r="11" spans="1:10" customFormat="1" ht="22.5" customHeight="1">
-      <x:c r="A11" s="45" t="s"/>
-      <x:c r="B11" s="66" t="s">
+      <x:c r="B11" s="56" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C11" s="66" t="s">
+      <x:c r="C11" s="56" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D11" s="66" t="s">
+      <x:c r="D11" s="56" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E11" s="66" t="s">
+      <x:c r="E11" s="56" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="F11" s="66" t="s">
+      <x:c r="F11" s="56" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="G11" s="67" t="s">
+      <x:c r="G11" s="57" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="H11" s="67" t="s">
+      <x:c r="H11" s="57" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="I11" s="67" t="s">
+      <x:c r="I11" s="57" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="J11" s="67" t="s">
+      <x:c r="J11" s="57" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A12" s="45" t="s"/>
-      <x:c r="B12" s="68" t="n">
+      <x:c r="B12" s="58" t="n">
         <x:v>1072</x:v>
       </x:c>
-      <x:c r="C12" s="69">
+      <x:c r="C12" s="59">
         <x:v>32609</x:v>
       </x:c>
-      <x:c r="D12" s="69">
+      <x:c r="D12" s="59">
         <x:v>32610</x:v>
       </x:c>
-      <x:c r="E12" s="70" t="s"/>
-      <x:c r="F12" s="70" t="s"/>
-      <x:c r="G12" s="70" t="s">
+      <x:c r="E12" s="60" t="s"/>
+      <x:c r="F12" s="60" t="s"/>
+      <x:c r="G12" s="60" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H12" s="71" t="n">
+      <x:c r="H12" s="61" t="n">
         <x:v>3596</x:v>
       </x:c>
-      <x:c r="I12" s="71" t="n">
+      <x:c r="I12" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J12" s="71" t="n">
+      <x:c r="J12" s="61" t="n">
         <x:v>3596</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A13" s="45" t="s"/>
-      <x:c r="B13" s="68" t="n">
+      <x:c r="B13" s="58" t="n">
         <x:v>1059</x:v>
       </x:c>
-      <x:c r="C13" s="69">
+      <x:c r="C13" s="59">
         <x:v>32563</x:v>
       </x:c>
-      <x:c r="D13" s="69">
+      <x:c r="D13" s="59">
         <x:v>32564</x:v>
       </x:c>
-      <x:c r="E13" s="70" t="s">
+      <x:c r="E13" s="60" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="F13" s="70" t="s">
+      <x:c r="F13" s="60" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="G13" s="70" t="s">
+      <x:c r="G13" s="60" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H13" s="71" t="n">
+      <x:c r="H13" s="61" t="n">
         <x:v>2150</x:v>
       </x:c>
-      <x:c r="I13" s="71" t="n">
+      <x:c r="I13" s="61" t="n">
         <x:v>8.5</x:v>
       </x:c>
-      <x:c r="J13" s="71" t="n">
+      <x:c r="J13" s="61" t="n">
         <x:v>2150</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:10" customFormat="1" ht="12" customHeight="1" outlineLevel="1">
-      <x:c r="A14" s="45" t="s"/>
-      <x:c r="B14" s="74" t="s"/>
-      <x:c r="C14" s="74" t="s"/>
-      <x:c r="D14" s="74" t="s"/>
-      <x:c r="E14" s="74" t="s"/>
-      <x:c r="F14" s="74" t="s"/>
-      <x:c r="G14" s="75" t="s">
+      <x:c r="B14" s="62" t="s"/>
+      <x:c r="C14" s="62" t="s"/>
+      <x:c r="D14" s="62" t="s"/>
+      <x:c r="E14" s="62" t="s"/>
+      <x:c r="F14" s="62" t="s"/>
+      <x:c r="G14" s="63" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="H14" s="76" t="s"/>
-      <x:c r="I14" s="74">
+      <x:c r="H14" s="64" t="s"/>
+      <x:c r="I14" s="62">
         <x:f>Subtotal(9,I12:I13)</x:f>
       </x:c>
-      <x:c r="J14" s="76">
+      <x:c r="J14" s="64">
         <x:f>Subtotal(9,J12:J13)</x:f>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A15" s="45" t="s"/>
-      <x:c r="B15" s="68" t="n">
+      <x:c r="B15" s="58" t="n">
         <x:v>1280</x:v>
       </x:c>
-      <x:c r="C15" s="69">
+      <x:c r="C15" s="59">
         <x:v>34694</x:v>
       </x:c>
-      <x:c r="D15" s="69">
+      <x:c r="D15" s="59">
         <x:v>34694</x:v>
       </x:c>
-      <x:c r="E15" s="70" t="s"/>
-      <x:c r="F15" s="70" t="s"/>
-      <x:c r="G15" s="70" t="s">
+      <x:c r="E15" s="60" t="s"/>
+      <x:c r="F15" s="60" t="s"/>
+      <x:c r="G15" s="60" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H15" s="71" t="n">
+      <x:c r="H15" s="61" t="n">
         <x:v>4317.75</x:v>
       </x:c>
-      <x:c r="I15" s="71" t="n">
+      <x:c r="I15" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J15" s="71" t="n">
+      <x:c r="J15" s="61" t="n">
         <x:v>4317.75</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:10" customFormat="1" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1">
-      <x:c r="A16" s="45" t="s"/>
-      <x:c r="B16" s="68" t="n">
+      <x:c r="B16" s="58" t="n">
         <x:v>1080</x:v>
       </x:c>
-      <x:c r="C16" s="69">
+      <x:c r="C16" s="59">
         <x:v>32633</x:v>
       </x:c>
-      <x:c r="D16" s="69">
+      <x:c r="D16" s="59">
         <x:v>32634</x:v>
       </x:c>
-      <x:c r="E16" s="70" t="s"/>
-      <x:c r="F16" s="70" t="s"/>
-      <x:c r="G16" s="70" t="s">
+      <x:c r="E16" s="60" t="s"/>
+      <x:c r="F16" s="60" t="s"/>
+      <x:c r="G16" s="60" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H16" s="71" t="n">
+      <x:c r="H16" s="61" t="n">
         <x:v>9634</x:v>
       </x:c>
-      <x:c r="I16" s="71" t="n">
+      <x:c r="I16" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J16" s="71" t="n">
+      <x:c r="J16" s="61" t="n">
         <x:v>9634</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A17" s="45" t="s"/>
-      <x:c r="B17" s="68" t="n">
+      <x:c r="B17" s="58" t="n">
         <x:v>1180</x:v>
       </x:c>
-      <x:c r="C17" s="69">
+      <x:c r="C17" s="59">
         <x:v>34552</x:v>
       </x:c>
-      <x:c r="D17" s="69">
+      <x:c r="D17" s="59">
         <x:v>34552</x:v>
       </x:c>
-      <x:c r="E17" s="70" t="s"/>
-      <x:c r="F17" s="70" t="s"/>
-      <x:c r="G17" s="70" t="s">
+      <x:c r="E17" s="60" t="s"/>
+      <x:c r="F17" s="60" t="s"/>
+      <x:c r="G17" s="60" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H17" s="71" t="n">
+      <x:c r="H17" s="61" t="n">
         <x:v>3640</x:v>
       </x:c>
-      <x:c r="I17" s="71" t="n">
+      <x:c r="I17" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J17" s="71" t="n">
+      <x:c r="J17" s="61" t="n">
         <x:v>3640</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:10" outlineLevel="1">
-      <x:c r="A18" s="45" t="s"/>
-      <x:c r="B18" s="74" t="s"/>
-      <x:c r="C18" s="74" t="s"/>
-      <x:c r="D18" s="74" t="s"/>
-      <x:c r="E18" s="74" t="s"/>
-      <x:c r="F18" s="74" t="s"/>
-      <x:c r="G18" s="75" t="s">
+      <x:c r="B18" s="62" t="s"/>
+      <x:c r="C18" s="62" t="s"/>
+      <x:c r="D18" s="62" t="s"/>
+      <x:c r="E18" s="62" t="s"/>
+      <x:c r="F18" s="62" t="s"/>
+      <x:c r="G18" s="63" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="H18" s="76" t="s"/>
-      <x:c r="I18" s="74">
+      <x:c r="H18" s="64" t="s"/>
+      <x:c r="I18" s="62">
         <x:f>Subtotal(9,I15:I17)</x:f>
       </x:c>
-      <x:c r="J18" s="76">
+      <x:c r="J18" s="64">
         <x:f>Subtotal(9,J15:J17)</x:f>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A19" s="45" t="s"/>
-      <x:c r="B19" s="68" t="n">
+      <x:c r="B19" s="58" t="n">
         <x:v>1105</x:v>
       </x:c>
-      <x:c r="C19" s="69">
+      <x:c r="C19" s="59">
         <x:v>33806</x:v>
       </x:c>
-      <x:c r="D19" s="69">
+      <x:c r="D19" s="59">
         <x:v>33806</x:v>
       </x:c>
-      <x:c r="E19" s="70" t="s"/>
-      <x:c r="F19" s="70" t="s"/>
-      <x:c r="G19" s="70" t="s">
+      <x:c r="E19" s="60" t="s"/>
+      <x:c r="F19" s="60" t="s"/>
+      <x:c r="G19" s="60" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="H19" s="71" t="n">
+      <x:c r="H19" s="61" t="n">
         <x:v>31219.95</x:v>
       </x:c>
-      <x:c r="I19" s="71" t="n">
+      <x:c r="I19" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J19" s="71" t="n">
+      <x:c r="J19" s="61" t="n">
         <x:v>31219.95</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A20" s="45" t="s"/>
-      <x:c r="B20" s="68" t="n">
+      <x:c r="B20" s="58" t="n">
         <x:v>1266</x:v>
       </x:c>
-      <x:c r="C20" s="69">
+      <x:c r="C20" s="59">
         <x:v>34683</x:v>
       </x:c>
-      <x:c r="D20" s="69">
+      <x:c r="D20" s="59">
         <x:v>34683</x:v>
       </x:c>
-      <x:c r="E20" s="70" t="s"/>
-      <x:c r="F20" s="70" t="s"/>
-      <x:c r="G20" s="70" t="s">
+      <x:c r="E20" s="60" t="s"/>
+      <x:c r="F20" s="60" t="s"/>
+      <x:c r="G20" s="60" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="H20" s="71" t="n">
+      <x:c r="H20" s="61" t="n">
         <x:v>6935</x:v>
       </x:c>
-      <x:c r="I20" s="71" t="n">
+      <x:c r="I20" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J20" s="71" t="n">
+      <x:c r="J20" s="61" t="n">
         <x:v>6935</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A21" s="45" t="s"/>
-      <x:c r="B21" s="68" t="n">
+      <x:c r="B21" s="58" t="n">
         <x:v>1005</x:v>
       </x:c>
-      <x:c r="C21" s="69">
+      <x:c r="C21" s="59">
         <x:v>32253</x:v>
       </x:c>
-      <x:c r="D21" s="69">
+      <x:c r="D21" s="59">
         <x:v>32163</x:v>
       </x:c>
-      <x:c r="E21" s="70" t="s"/>
-      <x:c r="F21" s="70" t="s"/>
-      <x:c r="G21" s="70" t="s">
+      <x:c r="E21" s="60" t="s"/>
+      <x:c r="F21" s="60" t="s"/>
+      <x:c r="G21" s="60" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="H21" s="71" t="n">
+      <x:c r="H21" s="61" t="n">
         <x:v>4807</x:v>
       </x:c>
-      <x:c r="I21" s="71" t="n">
+      <x:c r="I21" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J21" s="71" t="n">
+      <x:c r="J21" s="61" t="n">
         <x:v>4807</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A22" s="45" t="s"/>
-      <x:c r="B22" s="68" t="n">
+      <x:c r="B22" s="58" t="n">
         <x:v>1305</x:v>
       </x:c>
-      <x:c r="C22" s="69">
+      <x:c r="C22" s="59">
         <x:v>34719</x:v>
       </x:c>
-      <x:c r="D22" s="69">
+      <x:c r="D22" s="59">
         <x:v>34719</x:v>
       </x:c>
-      <x:c r="E22" s="70" t="s"/>
-      <x:c r="F22" s="70" t="s"/>
-      <x:c r="G22" s="70" t="s">
+      <x:c r="E22" s="60" t="s"/>
+      <x:c r="F22" s="60" t="s"/>
+      <x:c r="G22" s="60" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="H22" s="71" t="n">
+      <x:c r="H22" s="61" t="n">
         <x:v>3065</x:v>
       </x:c>
-      <x:c r="I22" s="71" t="n">
+      <x:c r="I22" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J22" s="71" t="n">
+      <x:c r="J22" s="61" t="n">
         <x:v>3065</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:10" outlineLevel="1">
-      <x:c r="A23" s="45" t="s"/>
-      <x:c r="B23" s="74" t="s"/>
-      <x:c r="C23" s="74" t="s"/>
-      <x:c r="D23" s="74" t="s"/>
-      <x:c r="E23" s="74" t="s"/>
-      <x:c r="F23" s="74" t="s"/>
-      <x:c r="G23" s="75" t="s">
+      <x:c r="B23" s="62" t="s"/>
+      <x:c r="C23" s="62" t="s"/>
+      <x:c r="D23" s="62" t="s"/>
+      <x:c r="E23" s="62" t="s"/>
+      <x:c r="F23" s="62" t="s"/>
+      <x:c r="G23" s="63" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="H23" s="76" t="s"/>
-      <x:c r="I23" s="74">
+      <x:c r="H23" s="64" t="s"/>
+      <x:c r="I23" s="62">
         <x:f>Subtotal(9,I19:I22)</x:f>
       </x:c>
-      <x:c r="J23" s="76">
+      <x:c r="J23" s="64">
         <x:f>Subtotal(9,J19:J22)</x:f>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:10">
-      <x:c r="A24" s="45" t="s"/>
-      <x:c r="B24" s="74" t="s">
+      <x:c r="B24" s="62" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C24" s="74" t="s"/>
-      <x:c r="D24" s="74" t="s"/>
-      <x:c r="E24" s="74" t="s"/>
-      <x:c r="F24" s="74" t="s"/>
-      <x:c r="G24" s="75" t="s"/>
-      <x:c r="H24" s="76" t="s"/>
-      <x:c r="I24" s="74">
+      <x:c r="C24" s="62" t="s"/>
+      <x:c r="D24" s="62" t="s"/>
+      <x:c r="E24" s="62" t="s"/>
+      <x:c r="F24" s="62" t="s"/>
+      <x:c r="G24" s="63" t="s"/>
+      <x:c r="H24" s="64" t="s"/>
+      <x:c r="I24" s="62">
         <x:f>Subtotal(9,I12:I22)</x:f>
       </x:c>
-      <x:c r="J24" s="76">
+      <x:c r="J24" s="64">
         <x:f>Subtotal(9,J12:J22)</x:f>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:10">
-      <x:c r="A25" s="45" t="s"/>
-      <x:c r="B25" s="65" t="s"/>
-      <x:c r="C25" s="65" t="s"/>
-      <x:c r="D25" s="65" t="s"/>
-      <x:c r="E25" s="65" t="s"/>
-      <x:c r="F25" s="65" t="s"/>
-      <x:c r="G25" s="65" t="s"/>
-      <x:c r="H25" s="65" t="s"/>
-      <x:c r="I25" s="65" t="s"/>
-      <x:c r="J25" s="65" t="s"/>
+      <x:c r="B25" s="55" t="s"/>
+      <x:c r="C25" s="55" t="s"/>
+      <x:c r="D25" s="55" t="s"/>
+      <x:c r="E25" s="55" t="s"/>
+      <x:c r="F25" s="55" t="s"/>
+      <x:c r="G25" s="55" t="s"/>
+      <x:c r="H25" s="55" t="s"/>
+      <x:c r="I25" s="55" t="s"/>
+      <x:c r="J25" s="55" t="s"/>
     </x:row>
     <x:row r="26" spans="1:10">
-      <x:c r="A26" s="45" t="s"/>
-      <x:c r="B26" s="50" t="s">
+      <x:c r="B26" s="49" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="E26" s="50" t="s">
+      <x:c r="E26" s="49" t="s">
         <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:10">
-      <x:c r="A27" s="45" t="s"/>
-      <x:c r="B27" s="72" t="s">
+      <x:c r="B27" s="65" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="C27" s="57" t="s"/>
-      <x:c r="D27" s="57" t="s"/>
-      <x:c r="E27" s="72" t="s">
+      <x:c r="C27" s="13" t="s"/>
+      <x:c r="D27" s="13" t="s"/>
+      <x:c r="E27" s="65" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="F27" s="73" t="s"/>
-      <x:c r="G27" s="45" t="s"/>
-      <x:c r="J27" s="45" t="s"/>
+      <x:c r="F27" s="66" t="s"/>
     </x:row>
   </x:sheetData>
   <x:phoneticPr fontId="0" type="noConversion"/>
-  <x:conditionalFormatting sqref="E19:G22">
+  <x:conditionalFormatting sqref="E12:G13 E15:G17 E19:G22">
     <x:cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
-      <x:formula>$G19="Visa"</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E12:G13">
-    <x:cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <x:formula>$G12="Visa"</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E15:G17">
-    <x:cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
-      <x:formula>$G15="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Update reference files (ZIP code was trimmed)
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Collapse.xlsx
+++ b/tests/Gauges/GroupTagTests_Collapse.xlsx
@@ -11,14 +11,14 @@
   </x:sheets>
   <x:definedNames>
     <x:definedName name="Orders">Sheet1!$A$12:$J$24</x:definedName>
-    <x:definedName name="Orders_tpl">Sheet1!$A$12:$J$13</x:definedName>
+    <x:definedName name="Orders_tpl">Sheet1!$A$12:$J$24</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <x:si>
     <x:t>Collapse outline</x:t>
   </x:si>
@@ -51,6 +51,9 @@
   </x:si>
   <x:si>
     <x:t>US Virgin Islands</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00820</x:t>
   </x:si>
   <x:si>
     <x:t>Order No</x:t>
@@ -1227,8 +1230,8 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="H9" s="64" t="s"/>
-      <x:c r="I9" s="63" t="n">
-        <x:v>820</x:v>
+      <x:c r="I9" s="63" t="s">
+        <x:v>11</x:v>
       </x:c>
       <x:c r="J9" s="64" t="s"/>
     </x:row>
@@ -1247,31 +1250,31 @@
     <x:row r="11" spans="1:10" customFormat="1" ht="22.5" customHeight="1">
       <x:c r="A11" s="45" t="s"/>
       <x:c r="B11" s="66" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C11" s="66" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D11" s="66" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E11" s="66" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F11" s="66" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="G11" s="67" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="H11" s="67" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="I11" s="67" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="J11" s="67" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
@@ -1288,7 +1291,7 @@
       <x:c r="E12" s="70" t="s"/>
       <x:c r="F12" s="70" t="s"/>
       <x:c r="G12" s="70" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H12" s="71" t="n">
         <x:v>3596</x:v>
@@ -1312,13 +1315,13 @@
         <x:v>32564</x:v>
       </x:c>
       <x:c r="E13" s="70" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F13" s="70" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G13" s="70" t="s">
         <x:v>21</x:v>
-      </x:c>
-      <x:c r="F13" s="70" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G13" s="70" t="s">
-        <x:v>20</x:v>
       </x:c>
       <x:c r="H13" s="71" t="n">
         <x:v>2150</x:v>
@@ -1338,7 +1341,7 @@
       <x:c r="E14" s="74" t="s"/>
       <x:c r="F14" s="74" t="s"/>
       <x:c r="G14" s="75" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H14" s="76" t="s"/>
       <x:c r="I14" s="74">
@@ -1362,7 +1365,7 @@
       <x:c r="E15" s="70" t="s"/>
       <x:c r="F15" s="70" t="s"/>
       <x:c r="G15" s="70" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H15" s="71" t="n">
         <x:v>4317.75</x:v>
@@ -1388,7 +1391,7 @@
       <x:c r="E16" s="70" t="s"/>
       <x:c r="F16" s="70" t="s"/>
       <x:c r="G16" s="70" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H16" s="71" t="n">
         <x:v>9634</x:v>
@@ -1414,7 +1417,7 @@
       <x:c r="E17" s="70" t="s"/>
       <x:c r="F17" s="70" t="s"/>
       <x:c r="G17" s="70" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H17" s="71" t="n">
         <x:v>3640</x:v>
@@ -1434,7 +1437,7 @@
       <x:c r="E18" s="74" t="s"/>
       <x:c r="F18" s="74" t="s"/>
       <x:c r="G18" s="75" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H18" s="76" t="s"/>
       <x:c r="I18" s="74">
@@ -1458,7 +1461,7 @@
       <x:c r="E19" s="70" t="s"/>
       <x:c r="F19" s="70" t="s"/>
       <x:c r="G19" s="70" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H19" s="71" t="n">
         <x:v>31219.95</x:v>
@@ -1484,7 +1487,7 @@
       <x:c r="E20" s="70" t="s"/>
       <x:c r="F20" s="70" t="s"/>
       <x:c r="G20" s="70" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H20" s="71" t="n">
         <x:v>6935</x:v>
@@ -1510,7 +1513,7 @@
       <x:c r="E21" s="70" t="s"/>
       <x:c r="F21" s="70" t="s"/>
       <x:c r="G21" s="70" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H21" s="71" t="n">
         <x:v>4807</x:v>
@@ -1536,7 +1539,7 @@
       <x:c r="E22" s="70" t="s"/>
       <x:c r="F22" s="70" t="s"/>
       <x:c r="G22" s="70" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H22" s="71" t="n">
         <x:v>3065</x:v>
@@ -1556,7 +1559,7 @@
       <x:c r="E23" s="74" t="s"/>
       <x:c r="F23" s="74" t="s"/>
       <x:c r="G23" s="75" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="H23" s="76" t="s"/>
       <x:c r="I23" s="74">
@@ -1569,7 +1572,7 @@
     <x:row r="24" spans="1:10">
       <x:c r="A24" s="45" t="s"/>
       <x:c r="B24" s="74" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C24" s="74" t="s"/>
       <x:c r="D24" s="74" t="s"/>
@@ -1599,21 +1602,21 @@
     <x:row r="26" spans="1:10">
       <x:c r="A26" s="45" t="s"/>
       <x:c r="B26" s="50" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E26" s="50" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:10">
       <x:c r="A27" s="45" t="s"/>
       <x:c r="B27" s="72" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C27" s="57" t="s"/>
       <x:c r="D27" s="57" t="s"/>
       <x:c r="E27" s="72" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F27" s="73" t="s"/>
       <x:c r="G27" s="45" t="s"/>

</xml_diff>

<commit_message>
Leading zeros are trimmed (#72)
* Add failing test for leading zeros

* Change the assignment of cell values so that leading zeros were not trimmed

* Update reference files (ZIP code was trimmed)
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Collapse.xlsx
+++ b/tests/Gauges/GroupTagTests_Collapse.xlsx
@@ -11,14 +11,14 @@
   </x:sheets>
   <x:definedNames>
     <x:definedName name="Orders">Sheet1!$A$12:$J$24</x:definedName>
-    <x:definedName name="Orders_tpl">Sheet1!$A$12:$J$13</x:definedName>
+    <x:definedName name="Orders_tpl">Sheet1!$A$12:$J$24</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <x:si>
     <x:t>Collapse outline</x:t>
   </x:si>
@@ -51,6 +51,9 @@
   </x:si>
   <x:si>
     <x:t>US Virgin Islands</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00820</x:t>
   </x:si>
   <x:si>
     <x:t>Order No</x:t>
@@ -1227,8 +1230,8 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="H9" s="64" t="s"/>
-      <x:c r="I9" s="63" t="n">
-        <x:v>820</x:v>
+      <x:c r="I9" s="63" t="s">
+        <x:v>11</x:v>
       </x:c>
       <x:c r="J9" s="64" t="s"/>
     </x:row>
@@ -1247,31 +1250,31 @@
     <x:row r="11" spans="1:10" customFormat="1" ht="22.5" customHeight="1">
       <x:c r="A11" s="45" t="s"/>
       <x:c r="B11" s="66" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C11" s="66" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D11" s="66" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E11" s="66" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F11" s="66" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="G11" s="67" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="H11" s="67" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="I11" s="67" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="J11" s="67" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
@@ -1288,7 +1291,7 @@
       <x:c r="E12" s="70" t="s"/>
       <x:c r="F12" s="70" t="s"/>
       <x:c r="G12" s="70" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H12" s="71" t="n">
         <x:v>3596</x:v>
@@ -1312,13 +1315,13 @@
         <x:v>32564</x:v>
       </x:c>
       <x:c r="E13" s="70" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F13" s="70" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G13" s="70" t="s">
         <x:v>21</x:v>
-      </x:c>
-      <x:c r="F13" s="70" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G13" s="70" t="s">
-        <x:v>20</x:v>
       </x:c>
       <x:c r="H13" s="71" t="n">
         <x:v>2150</x:v>
@@ -1338,7 +1341,7 @@
       <x:c r="E14" s="74" t="s"/>
       <x:c r="F14" s="74" t="s"/>
       <x:c r="G14" s="75" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H14" s="76" t="s"/>
       <x:c r="I14" s="74">
@@ -1362,7 +1365,7 @@
       <x:c r="E15" s="70" t="s"/>
       <x:c r="F15" s="70" t="s"/>
       <x:c r="G15" s="70" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H15" s="71" t="n">
         <x:v>4317.75</x:v>
@@ -1388,7 +1391,7 @@
       <x:c r="E16" s="70" t="s"/>
       <x:c r="F16" s="70" t="s"/>
       <x:c r="G16" s="70" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H16" s="71" t="n">
         <x:v>9634</x:v>
@@ -1414,7 +1417,7 @@
       <x:c r="E17" s="70" t="s"/>
       <x:c r="F17" s="70" t="s"/>
       <x:c r="G17" s="70" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="H17" s="71" t="n">
         <x:v>3640</x:v>
@@ -1434,7 +1437,7 @@
       <x:c r="E18" s="74" t="s"/>
       <x:c r="F18" s="74" t="s"/>
       <x:c r="G18" s="75" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H18" s="76" t="s"/>
       <x:c r="I18" s="74">
@@ -1458,7 +1461,7 @@
       <x:c r="E19" s="70" t="s"/>
       <x:c r="F19" s="70" t="s"/>
       <x:c r="G19" s="70" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H19" s="71" t="n">
         <x:v>31219.95</x:v>
@@ -1484,7 +1487,7 @@
       <x:c r="E20" s="70" t="s"/>
       <x:c r="F20" s="70" t="s"/>
       <x:c r="G20" s="70" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H20" s="71" t="n">
         <x:v>6935</x:v>
@@ -1510,7 +1513,7 @@
       <x:c r="E21" s="70" t="s"/>
       <x:c r="F21" s="70" t="s"/>
       <x:c r="G21" s="70" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H21" s="71" t="n">
         <x:v>4807</x:v>
@@ -1536,7 +1539,7 @@
       <x:c r="E22" s="70" t="s"/>
       <x:c r="F22" s="70" t="s"/>
       <x:c r="G22" s="70" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H22" s="71" t="n">
         <x:v>3065</x:v>
@@ -1556,7 +1559,7 @@
       <x:c r="E23" s="74" t="s"/>
       <x:c r="F23" s="74" t="s"/>
       <x:c r="G23" s="75" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="H23" s="76" t="s"/>
       <x:c r="I23" s="74">
@@ -1569,7 +1572,7 @@
     <x:row r="24" spans="1:10">
       <x:c r="A24" s="45" t="s"/>
       <x:c r="B24" s="74" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C24" s="74" t="s"/>
       <x:c r="D24" s="74" t="s"/>
@@ -1599,21 +1602,21 @@
     <x:row r="26" spans="1:10">
       <x:c r="A26" s="45" t="s"/>
       <x:c r="B26" s="50" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E26" s="50" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:10">
       <x:c r="A27" s="45" t="s"/>
       <x:c r="B27" s="72" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C27" s="57" t="s"/>
       <x:c r="D27" s="57" t="s"/>
       <x:c r="E27" s="72" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F27" s="73" t="s"/>
       <x:c r="G27" s="45" t="s"/>

</xml_diff>

<commit_message>
Upgrade to ClosedXML 0.95 (#73)
Great work, thanks Alexey.
I will make my small edits and it will be possible to make a release.

* Upgrade ClosedXML to 0.95.0-beta1. Fix compilation issues
* Modify code according to changes in ClosedXML 0.95
* Remove obsolete code
* Upgrade a reference file: consolidate conditional formats and other minor changes
* Use pattern matching and other small refactoring
* Upgrade xUnit version
* Bump version to 0.2.0
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Collapse.xlsx
+++ b/tests/Gauges/GroupTagTests_Collapse.xlsx
@@ -309,11 +309,8 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="23">
+  <x:cellStyleXfs count="22">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -368,17 +365,17 @@
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="77">
+  <x:cellXfs count="67">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -486,10 +483,6 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <x:xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -510,46 +503,14 @@
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -558,10 +519,6 @@
       <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -594,24 +551,24 @@
       <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="12" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -621,10 +578,6 @@
   <x:dxfs count="1">
     <x:dxf>
       <x:font>
-        <x:b val="0"/>
-        <x:i val="0"/>
-        <x:condense val="0"/>
-        <x:extend val="0"/>
         <x:color indexed="30"/>
       </x:font>
     </x:dxf>
@@ -711,9 +664,9 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1695450" cy="609600"/>
+    <xdr:ext cx="1699260" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Рисунок 2"/>
@@ -730,7 +683,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1695450" cy="609600"/>
+          <a:ext cx="1699260" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
       </xdr:spPr>
@@ -1101,542 +1054,492 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="2"/>
   <x:cols>
-    <x:col min="1" max="1" width="2.832031" style="45" customWidth="1"/>
-    <x:col min="2" max="2" width="9" style="45" customWidth="1"/>
-    <x:col min="3" max="3" width="9.664062" style="45" customWidth="1"/>
-    <x:col min="4" max="4" width="9.140625" style="45" customWidth="1"/>
-    <x:col min="5" max="5" width="6.164062" style="45" customWidth="1"/>
-    <x:col min="6" max="6" width="6.832031" style="45" customWidth="1"/>
-    <x:col min="7" max="7" width="8.5" style="45" customWidth="1"/>
-    <x:col min="8" max="8" width="9.164062" style="45" customWidth="1"/>
-    <x:col min="9" max="9" width="7.332031" style="45" customWidth="1"/>
-    <x:col min="10" max="10" width="11.5" style="45" customWidth="1"/>
+    <x:col min="1" max="1" width="2.832031" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="9" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="9.664062" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="6.164062" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="6.832031" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="8.5" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="9.164062" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="7.332031" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="11.5" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:10" customFormat="1" ht="51" customHeight="1">
-      <x:c r="A1" s="45" t="s"/>
-      <x:c r="B1" s="46" t="s">
+      <x:c r="B1" s="45" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C1" s="47" t="s"/>
-      <x:c r="D1" s="47" t="s"/>
-      <x:c r="E1" s="47" t="s"/>
-      <x:c r="F1" s="47" t="s"/>
-      <x:c r="G1" s="47" t="s"/>
-      <x:c r="H1" s="47" t="s"/>
-      <x:c r="I1" s="47" t="s"/>
-      <x:c r="J1" s="47" t="s"/>
+      <x:c r="C1" s="46" t="s"/>
+      <x:c r="D1" s="46" t="s"/>
+      <x:c r="E1" s="46" t="s"/>
+      <x:c r="F1" s="46" t="s"/>
+      <x:c r="G1" s="46" t="s"/>
+      <x:c r="H1" s="46" t="s"/>
+      <x:c r="I1" s="46" t="s"/>
+      <x:c r="J1" s="46" t="s"/>
     </x:row>
     <x:row r="2" spans="1:10" customFormat="1" ht="12.75" customHeight="1">
-      <x:c r="A2" s="45" t="s"/>
-      <x:c r="B2" s="48" t="s"/>
-      <x:c r="C2" s="48" t="s"/>
-      <x:c r="D2" s="48" t="s"/>
-      <x:c r="E2" s="48" t="s"/>
-      <x:c r="F2" s="48" t="s"/>
-      <x:c r="G2" s="48" t="s"/>
-      <x:c r="H2" s="48" t="s"/>
-      <x:c r="I2" s="48" t="s"/>
-      <x:c r="J2" s="45" t="s"/>
+      <x:c r="B2" s="47" t="s"/>
+      <x:c r="C2" s="47" t="s"/>
+      <x:c r="D2" s="47" t="s"/>
+      <x:c r="E2" s="47" t="s"/>
+      <x:c r="F2" s="47" t="s"/>
+      <x:c r="G2" s="47" t="s"/>
+      <x:c r="H2" s="47" t="s"/>
+      <x:c r="I2" s="47" t="s"/>
     </x:row>
     <x:row r="3" spans="1:10" customFormat="1" ht="18" customHeight="1">
-      <x:c r="A3" s="49" t="s"/>
-      <x:c r="B3" s="50" t="s">
+      <x:c r="A3" s="48" t="s"/>
+      <x:c r="B3" s="49" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="51" t="s">
+      <x:c r="C3" s="32" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D3" s="52" t="s"/>
-      <x:c r="E3" s="52" t="s"/>
-      <x:c r="F3" s="52" t="s"/>
-      <x:c r="G3" s="53" t="s"/>
-      <x:c r="H3" s="53" t="s"/>
-      <x:c r="I3" s="53" t="s"/>
-      <x:c r="J3" s="54" t="s"/>
+      <x:c r="D3" s="21" t="s"/>
+      <x:c r="E3" s="21" t="s"/>
+      <x:c r="F3" s="21" t="s"/>
+      <x:c r="G3" s="17" t="s"/>
+      <x:c r="H3" s="17" t="s"/>
+      <x:c r="I3" s="17" t="s"/>
+      <x:c r="J3" s="18" t="s"/>
     </x:row>
     <x:row r="4" spans="1:10">
-      <x:c r="A4" s="45" t="s"/>
-      <x:c r="B4" s="55" t="s"/>
-      <x:c r="C4" s="45" t="s"/>
-      <x:c r="D4" s="45" t="s"/>
-      <x:c r="E4" s="45" t="s"/>
-      <x:c r="F4" s="45" t="s"/>
-      <x:c r="G4" s="45" t="s"/>
-      <x:c r="H4" s="45" t="s"/>
-      <x:c r="I4" s="45" t="s"/>
-      <x:c r="J4" s="45" t="s"/>
+      <x:c r="B4" s="50" t="s"/>
     </x:row>
     <x:row r="5" spans="1:10">
-      <x:c r="A5" s="45" t="s"/>
-      <x:c r="B5" s="50" t="s">
+      <x:c r="B5" s="49" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C5" s="45" t="s"/>
     </x:row>
     <x:row r="6" spans="1:10" customFormat="1" ht="12" customHeight="1">
-      <x:c r="A6" s="45" t="s"/>
-      <x:c r="B6" s="56" t="s">
+      <x:c r="B6" s="42" t="s">
         <x:f>"632-1 Third Frydenhoj"&amp;" "&amp;""</x:f>
       </x:c>
-      <x:c r="C6" s="57" t="s"/>
-      <x:c r="D6" s="57" t="s"/>
-      <x:c r="E6" s="57" t="s"/>
-      <x:c r="F6" s="57" t="s"/>
-      <x:c r="G6" s="57" t="s"/>
-      <x:c r="H6" s="58" t="s"/>
-      <x:c r="I6" s="59" t="s"/>
-      <x:c r="J6" s="60" t="s"/>
+      <x:c r="C6" s="13" t="s"/>
+      <x:c r="D6" s="13" t="s"/>
+      <x:c r="E6" s="13" t="s"/>
+      <x:c r="F6" s="13" t="s"/>
+      <x:c r="G6" s="13" t="s"/>
+      <x:c r="H6" s="51" t="s"/>
+      <x:c r="I6" s="15" t="s"/>
+      <x:c r="J6" s="16" t="s"/>
     </x:row>
     <x:row r="7" spans="1:10" customFormat="1" ht="12" customHeight="1">
-      <x:c r="A7" s="45" t="s"/>
-      <x:c r="B7" s="61" t="s"/>
-      <x:c r="C7" s="62" t="s"/>
-      <x:c r="D7" s="62" t="s"/>
-      <x:c r="E7" s="62" t="s"/>
-      <x:c r="F7" s="62" t="s"/>
-      <x:c r="G7" s="62" t="s"/>
-      <x:c r="H7" s="61" t="s"/>
-      <x:c r="I7" s="45" t="s"/>
-      <x:c r="J7" s="45" t="s"/>
+      <x:c r="B7" s="52" t="s"/>
+      <x:c r="C7" s="53" t="s"/>
+      <x:c r="D7" s="53" t="s"/>
+      <x:c r="E7" s="53" t="s"/>
+      <x:c r="F7" s="53" t="s"/>
+      <x:c r="G7" s="53" t="s"/>
+      <x:c r="H7" s="52" t="s"/>
     </x:row>
     <x:row r="8" spans="1:10">
-      <x:c r="A8" s="45" t="s"/>
-      <x:c r="B8" s="50" t="s">
+      <x:c r="B8" s="49" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="E8" s="50" t="s">
+      <x:c r="E8" s="49" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G8" s="50" t="s">
+      <x:c r="G8" s="49" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="I8" s="50" t="s">
+      <x:c r="I8" s="49" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10" customFormat="1" ht="12" customHeight="1">
-      <x:c r="A9" s="45" t="s"/>
-      <x:c r="B9" s="63" t="s">
+      <x:c r="B9" s="35" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C9" s="57" t="s"/>
-      <x:c r="D9" s="57" t="s"/>
-      <x:c r="E9" s="63" t="s">
+      <x:c r="C9" s="13" t="s"/>
+      <x:c r="D9" s="13" t="s"/>
+      <x:c r="E9" s="35" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F9" s="64" t="s"/>
-      <x:c r="G9" s="63" t="s">
+      <x:c r="F9" s="54" t="s"/>
+      <x:c r="G9" s="35" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="H9" s="64" t="s"/>
-      <x:c r="I9" s="63" t="s">
+      <x:c r="H9" s="54" t="s"/>
+      <x:c r="I9" s="35" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="J9" s="64" t="s"/>
+      <x:c r="J9" s="54" t="s"/>
     </x:row>
     <x:row r="10" spans="1:10" customFormat="1" ht="12" customHeight="1">
-      <x:c r="A10" s="45" t="s"/>
-      <x:c r="B10" s="65" t="s"/>
-      <x:c r="C10" s="65" t="s"/>
-      <x:c r="D10" s="65" t="s"/>
-      <x:c r="E10" s="65" t="s"/>
-      <x:c r="F10" s="65" t="s"/>
-      <x:c r="G10" s="65" t="s"/>
-      <x:c r="H10" s="65" t="s"/>
-      <x:c r="I10" s="65" t="s"/>
-      <x:c r="J10" s="65" t="s"/>
+      <x:c r="B10" s="55" t="s"/>
+      <x:c r="C10" s="55" t="s"/>
+      <x:c r="D10" s="55" t="s"/>
+      <x:c r="E10" s="55" t="s"/>
+      <x:c r="F10" s="55" t="s"/>
+      <x:c r="G10" s="55" t="s"/>
+      <x:c r="H10" s="55" t="s"/>
+      <x:c r="I10" s="55" t="s"/>
+      <x:c r="J10" s="55" t="s"/>
     </x:row>
     <x:row r="11" spans="1:10" customFormat="1" ht="22.5" customHeight="1">
-      <x:c r="A11" s="45" t="s"/>
-      <x:c r="B11" s="66" t="s">
+      <x:c r="B11" s="56" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C11" s="66" t="s">
+      <x:c r="C11" s="56" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D11" s="66" t="s">
+      <x:c r="D11" s="56" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E11" s="66" t="s">
+      <x:c r="E11" s="56" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="F11" s="66" t="s">
+      <x:c r="F11" s="56" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="G11" s="67" t="s">
+      <x:c r="G11" s="57" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="H11" s="67" t="s">
+      <x:c r="H11" s="57" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="I11" s="67" t="s">
+      <x:c r="I11" s="57" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="J11" s="67" t="s">
+      <x:c r="J11" s="57" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A12" s="45" t="s"/>
-      <x:c r="B12" s="68" t="n">
+      <x:c r="B12" s="58" t="n">
         <x:v>1072</x:v>
       </x:c>
-      <x:c r="C12" s="69">
+      <x:c r="C12" s="59">
         <x:v>32609</x:v>
       </x:c>
-      <x:c r="D12" s="69">
+      <x:c r="D12" s="59">
         <x:v>32610</x:v>
       </x:c>
-      <x:c r="E12" s="70" t="s"/>
-      <x:c r="F12" s="70" t="s"/>
-      <x:c r="G12" s="70" t="s">
+      <x:c r="E12" s="60" t="s"/>
+      <x:c r="F12" s="60" t="s"/>
+      <x:c r="G12" s="60" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H12" s="71" t="n">
+      <x:c r="H12" s="61" t="n">
         <x:v>3596</x:v>
       </x:c>
-      <x:c r="I12" s="71" t="n">
+      <x:c r="I12" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J12" s="71" t="n">
+      <x:c r="J12" s="61" t="n">
         <x:v>3596</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A13" s="45" t="s"/>
-      <x:c r="B13" s="68" t="n">
+      <x:c r="B13" s="58" t="n">
         <x:v>1059</x:v>
       </x:c>
-      <x:c r="C13" s="69">
+      <x:c r="C13" s="59">
         <x:v>32563</x:v>
       </x:c>
-      <x:c r="D13" s="69">
+      <x:c r="D13" s="59">
         <x:v>32564</x:v>
       </x:c>
-      <x:c r="E13" s="70" t="s">
+      <x:c r="E13" s="60" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="F13" s="70" t="s">
+      <x:c r="F13" s="60" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="G13" s="70" t="s">
+      <x:c r="G13" s="60" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H13" s="71" t="n">
+      <x:c r="H13" s="61" t="n">
         <x:v>2150</x:v>
       </x:c>
-      <x:c r="I13" s="71" t="n">
+      <x:c r="I13" s="61" t="n">
         <x:v>8.5</x:v>
       </x:c>
-      <x:c r="J13" s="71" t="n">
+      <x:c r="J13" s="61" t="n">
         <x:v>2150</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:10" customFormat="1" ht="12" customHeight="1" outlineLevel="1">
-      <x:c r="A14" s="45" t="s"/>
-      <x:c r="B14" s="74" t="s"/>
-      <x:c r="C14" s="74" t="s"/>
-      <x:c r="D14" s="74" t="s"/>
-      <x:c r="E14" s="74" t="s"/>
-      <x:c r="F14" s="74" t="s"/>
-      <x:c r="G14" s="75" t="s">
+      <x:c r="B14" s="62" t="s"/>
+      <x:c r="C14" s="62" t="s"/>
+      <x:c r="D14" s="62" t="s"/>
+      <x:c r="E14" s="62" t="s"/>
+      <x:c r="F14" s="62" t="s"/>
+      <x:c r="G14" s="63" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="H14" s="76" t="s"/>
-      <x:c r="I14" s="74">
+      <x:c r="H14" s="64" t="s"/>
+      <x:c r="I14" s="62">
         <x:f>Subtotal(9,I12:I13)</x:f>
       </x:c>
-      <x:c r="J14" s="76">
+      <x:c r="J14" s="64">
         <x:f>Subtotal(9,J12:J13)</x:f>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A15" s="45" t="s"/>
-      <x:c r="B15" s="68" t="n">
+      <x:c r="B15" s="58" t="n">
         <x:v>1280</x:v>
       </x:c>
-      <x:c r="C15" s="69">
+      <x:c r="C15" s="59">
         <x:v>34694</x:v>
       </x:c>
-      <x:c r="D15" s="69">
+      <x:c r="D15" s="59">
         <x:v>34694</x:v>
       </x:c>
-      <x:c r="E15" s="70" t="s"/>
-      <x:c r="F15" s="70" t="s"/>
-      <x:c r="G15" s="70" t="s">
+      <x:c r="E15" s="60" t="s"/>
+      <x:c r="F15" s="60" t="s"/>
+      <x:c r="G15" s="60" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H15" s="71" t="n">
+      <x:c r="H15" s="61" t="n">
         <x:v>4317.75</x:v>
       </x:c>
-      <x:c r="I15" s="71" t="n">
+      <x:c r="I15" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J15" s="71" t="n">
+      <x:c r="J15" s="61" t="n">
         <x:v>4317.75</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:10" customFormat="1" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1">
-      <x:c r="A16" s="45" t="s"/>
-      <x:c r="B16" s="68" t="n">
+      <x:c r="B16" s="58" t="n">
         <x:v>1080</x:v>
       </x:c>
-      <x:c r="C16" s="69">
+      <x:c r="C16" s="59">
         <x:v>32633</x:v>
       </x:c>
-      <x:c r="D16" s="69">
+      <x:c r="D16" s="59">
         <x:v>32634</x:v>
       </x:c>
-      <x:c r="E16" s="70" t="s"/>
-      <x:c r="F16" s="70" t="s"/>
-      <x:c r="G16" s="70" t="s">
+      <x:c r="E16" s="60" t="s"/>
+      <x:c r="F16" s="60" t="s"/>
+      <x:c r="G16" s="60" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H16" s="71" t="n">
+      <x:c r="H16" s="61" t="n">
         <x:v>9634</x:v>
       </x:c>
-      <x:c r="I16" s="71" t="n">
+      <x:c r="I16" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J16" s="71" t="n">
+      <x:c r="J16" s="61" t="n">
         <x:v>9634</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A17" s="45" t="s"/>
-      <x:c r="B17" s="68" t="n">
+      <x:c r="B17" s="58" t="n">
         <x:v>1180</x:v>
       </x:c>
-      <x:c r="C17" s="69">
+      <x:c r="C17" s="59">
         <x:v>34552</x:v>
       </x:c>
-      <x:c r="D17" s="69">
+      <x:c r="D17" s="59">
         <x:v>34552</x:v>
       </x:c>
-      <x:c r="E17" s="70" t="s"/>
-      <x:c r="F17" s="70" t="s"/>
-      <x:c r="G17" s="70" t="s">
+      <x:c r="E17" s="60" t="s"/>
+      <x:c r="F17" s="60" t="s"/>
+      <x:c r="G17" s="60" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H17" s="71" t="n">
+      <x:c r="H17" s="61" t="n">
         <x:v>3640</x:v>
       </x:c>
-      <x:c r="I17" s="71" t="n">
+      <x:c r="I17" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J17" s="71" t="n">
+      <x:c r="J17" s="61" t="n">
         <x:v>3640</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:10" outlineLevel="1">
-      <x:c r="A18" s="45" t="s"/>
-      <x:c r="B18" s="74" t="s"/>
-      <x:c r="C18" s="74" t="s"/>
-      <x:c r="D18" s="74" t="s"/>
-      <x:c r="E18" s="74" t="s"/>
-      <x:c r="F18" s="74" t="s"/>
-      <x:c r="G18" s="75" t="s">
+      <x:c r="B18" s="62" t="s"/>
+      <x:c r="C18" s="62" t="s"/>
+      <x:c r="D18" s="62" t="s"/>
+      <x:c r="E18" s="62" t="s"/>
+      <x:c r="F18" s="62" t="s"/>
+      <x:c r="G18" s="63" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="H18" s="76" t="s"/>
-      <x:c r="I18" s="74">
+      <x:c r="H18" s="64" t="s"/>
+      <x:c r="I18" s="62">
         <x:f>Subtotal(9,I15:I17)</x:f>
       </x:c>
-      <x:c r="J18" s="76">
+      <x:c r="J18" s="64">
         <x:f>Subtotal(9,J15:J17)</x:f>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A19" s="45" t="s"/>
-      <x:c r="B19" s="68" t="n">
+      <x:c r="B19" s="58" t="n">
         <x:v>1105</x:v>
       </x:c>
-      <x:c r="C19" s="69">
+      <x:c r="C19" s="59">
         <x:v>33806</x:v>
       </x:c>
-      <x:c r="D19" s="69">
+      <x:c r="D19" s="59">
         <x:v>33806</x:v>
       </x:c>
-      <x:c r="E19" s="70" t="s"/>
-      <x:c r="F19" s="70" t="s"/>
-      <x:c r="G19" s="70" t="s">
+      <x:c r="E19" s="60" t="s"/>
+      <x:c r="F19" s="60" t="s"/>
+      <x:c r="G19" s="60" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="H19" s="71" t="n">
+      <x:c r="H19" s="61" t="n">
         <x:v>31219.95</x:v>
       </x:c>
-      <x:c r="I19" s="71" t="n">
+      <x:c r="I19" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J19" s="71" t="n">
+      <x:c r="J19" s="61" t="n">
         <x:v>31219.95</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A20" s="45" t="s"/>
-      <x:c r="B20" s="68" t="n">
+      <x:c r="B20" s="58" t="n">
         <x:v>1266</x:v>
       </x:c>
-      <x:c r="C20" s="69">
+      <x:c r="C20" s="59">
         <x:v>34683</x:v>
       </x:c>
-      <x:c r="D20" s="69">
+      <x:c r="D20" s="59">
         <x:v>34683</x:v>
       </x:c>
-      <x:c r="E20" s="70" t="s"/>
-      <x:c r="F20" s="70" t="s"/>
-      <x:c r="G20" s="70" t="s">
+      <x:c r="E20" s="60" t="s"/>
+      <x:c r="F20" s="60" t="s"/>
+      <x:c r="G20" s="60" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="H20" s="71" t="n">
+      <x:c r="H20" s="61" t="n">
         <x:v>6935</x:v>
       </x:c>
-      <x:c r="I20" s="71" t="n">
+      <x:c r="I20" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J20" s="71" t="n">
+      <x:c r="J20" s="61" t="n">
         <x:v>6935</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A21" s="45" t="s"/>
-      <x:c r="B21" s="68" t="n">
+      <x:c r="B21" s="58" t="n">
         <x:v>1005</x:v>
       </x:c>
-      <x:c r="C21" s="69">
+      <x:c r="C21" s="59">
         <x:v>32253</x:v>
       </x:c>
-      <x:c r="D21" s="69">
+      <x:c r="D21" s="59">
         <x:v>32163</x:v>
       </x:c>
-      <x:c r="E21" s="70" t="s"/>
-      <x:c r="F21" s="70" t="s"/>
-      <x:c r="G21" s="70" t="s">
+      <x:c r="E21" s="60" t="s"/>
+      <x:c r="F21" s="60" t="s"/>
+      <x:c r="G21" s="60" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="H21" s="71" t="n">
+      <x:c r="H21" s="61" t="n">
         <x:v>4807</x:v>
       </x:c>
-      <x:c r="I21" s="71" t="n">
+      <x:c r="I21" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J21" s="71" t="n">
+      <x:c r="J21" s="61" t="n">
         <x:v>4807</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:10" hidden="1" outlineLevel="2" collapsed="1">
-      <x:c r="A22" s="45" t="s"/>
-      <x:c r="B22" s="68" t="n">
+      <x:c r="B22" s="58" t="n">
         <x:v>1305</x:v>
       </x:c>
-      <x:c r="C22" s="69">
+      <x:c r="C22" s="59">
         <x:v>34719</x:v>
       </x:c>
-      <x:c r="D22" s="69">
+      <x:c r="D22" s="59">
         <x:v>34719</x:v>
       </x:c>
-      <x:c r="E22" s="70" t="s"/>
-      <x:c r="F22" s="70" t="s"/>
-      <x:c r="G22" s="70" t="s">
+      <x:c r="E22" s="60" t="s"/>
+      <x:c r="F22" s="60" t="s"/>
+      <x:c r="G22" s="60" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="H22" s="71" t="n">
+      <x:c r="H22" s="61" t="n">
         <x:v>3065</x:v>
       </x:c>
-      <x:c r="I22" s="71" t="n">
+      <x:c r="I22" s="61" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J22" s="71" t="n">
+      <x:c r="J22" s="61" t="n">
         <x:v>3065</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:10" outlineLevel="1">
-      <x:c r="A23" s="45" t="s"/>
-      <x:c r="B23" s="74" t="s"/>
-      <x:c r="C23" s="74" t="s"/>
-      <x:c r="D23" s="74" t="s"/>
-      <x:c r="E23" s="74" t="s"/>
-      <x:c r="F23" s="74" t="s"/>
-      <x:c r="G23" s="75" t="s">
+      <x:c r="B23" s="62" t="s"/>
+      <x:c r="C23" s="62" t="s"/>
+      <x:c r="D23" s="62" t="s"/>
+      <x:c r="E23" s="62" t="s"/>
+      <x:c r="F23" s="62" t="s"/>
+      <x:c r="G23" s="63" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="H23" s="76" t="s"/>
-      <x:c r="I23" s="74">
+      <x:c r="H23" s="64" t="s"/>
+      <x:c r="I23" s="62">
         <x:f>Subtotal(9,I19:I22)</x:f>
       </x:c>
-      <x:c r="J23" s="76">
+      <x:c r="J23" s="64">
         <x:f>Subtotal(9,J19:J22)</x:f>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:10">
-      <x:c r="A24" s="45" t="s"/>
-      <x:c r="B24" s="74" t="s">
+      <x:c r="B24" s="62" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C24" s="74" t="s"/>
-      <x:c r="D24" s="74" t="s"/>
-      <x:c r="E24" s="74" t="s"/>
-      <x:c r="F24" s="74" t="s"/>
-      <x:c r="G24" s="75" t="s"/>
-      <x:c r="H24" s="76" t="s"/>
-      <x:c r="I24" s="74">
+      <x:c r="C24" s="62" t="s"/>
+      <x:c r="D24" s="62" t="s"/>
+      <x:c r="E24" s="62" t="s"/>
+      <x:c r="F24" s="62" t="s"/>
+      <x:c r="G24" s="63" t="s"/>
+      <x:c r="H24" s="64" t="s"/>
+      <x:c r="I24" s="62">
         <x:f>Subtotal(9,I12:I22)</x:f>
       </x:c>
-      <x:c r="J24" s="76">
+      <x:c r="J24" s="64">
         <x:f>Subtotal(9,J12:J22)</x:f>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:10">
-      <x:c r="A25" s="45" t="s"/>
-      <x:c r="B25" s="65" t="s"/>
-      <x:c r="C25" s="65" t="s"/>
-      <x:c r="D25" s="65" t="s"/>
-      <x:c r="E25" s="65" t="s"/>
-      <x:c r="F25" s="65" t="s"/>
-      <x:c r="G25" s="65" t="s"/>
-      <x:c r="H25" s="65" t="s"/>
-      <x:c r="I25" s="65" t="s"/>
-      <x:c r="J25" s="65" t="s"/>
+      <x:c r="B25" s="55" t="s"/>
+      <x:c r="C25" s="55" t="s"/>
+      <x:c r="D25" s="55" t="s"/>
+      <x:c r="E25" s="55" t="s"/>
+      <x:c r="F25" s="55" t="s"/>
+      <x:c r="G25" s="55" t="s"/>
+      <x:c r="H25" s="55" t="s"/>
+      <x:c r="I25" s="55" t="s"/>
+      <x:c r="J25" s="55" t="s"/>
     </x:row>
     <x:row r="26" spans="1:10">
-      <x:c r="A26" s="45" t="s"/>
-      <x:c r="B26" s="50" t="s">
+      <x:c r="B26" s="49" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="E26" s="50" t="s">
+      <x:c r="E26" s="49" t="s">
         <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:10">
-      <x:c r="A27" s="45" t="s"/>
-      <x:c r="B27" s="72" t="s">
+      <x:c r="B27" s="65" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="C27" s="57" t="s"/>
-      <x:c r="D27" s="57" t="s"/>
-      <x:c r="E27" s="72" t="s">
+      <x:c r="C27" s="13" t="s"/>
+      <x:c r="D27" s="13" t="s"/>
+      <x:c r="E27" s="65" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="F27" s="73" t="s"/>
-      <x:c r="G27" s="45" t="s"/>
-      <x:c r="J27" s="45" t="s"/>
+      <x:c r="F27" s="66" t="s"/>
     </x:row>
   </x:sheetData>
   <x:phoneticPr fontId="0" type="noConversion"/>
-  <x:conditionalFormatting sqref="E19:G22">
+  <x:conditionalFormatting sqref="E12:G13 E15:G17 E19:G22">
     <x:cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
-      <x:formula>$G19="Visa"</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E12:G13">
-    <x:cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <x:formula>$G12="Visa"</x:formula>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="E15:G17">
-    <x:cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
-      <x:formula>$G15="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>